<commit_message>
initial work to set stage for production of settlers and settlign new villages
</commit_message>
<xml_diff>
--- a/Raw_Building_Data.xlsx
+++ b/Raw_Building_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pyeac\Desktop\Travian Sim V2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{802BD1E8-4E89-4A1A-9A8E-09CDDA0BFB1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7933862-66C7-4ACC-B34E-DC61D7B67FBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{D964349E-A6D7-42EF-9507-D8E4572606D0}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="60">
   <si>
     <t>Building</t>
   </si>
@@ -2864,10 +2864,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{559C895B-DEBC-4F15-AD65-1EAADE192C37}">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3704,6 +3704,326 @@
         <v>0.25</v>
       </c>
     </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>580</v>
+      </c>
+      <c r="D27">
+        <v>460</v>
+      </c>
+      <c r="E27">
+        <v>350</v>
+      </c>
+      <c r="F27">
+        <v>180</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>2</v>
+      </c>
+      <c r="I27" s="1">
+        <v>2.3148148148148147E-2</v>
+      </c>
+      <c r="J27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28">
+        <v>740</v>
+      </c>
+      <c r="D28">
+        <v>590</v>
+      </c>
+      <c r="E28">
+        <v>450</v>
+      </c>
+      <c r="F28">
+        <v>230</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <v>3</v>
+      </c>
+      <c r="I28" s="1">
+        <v>3.0324074074074073E-2</v>
+      </c>
+      <c r="J28">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29">
+        <v>950</v>
+      </c>
+      <c r="D29">
+        <v>755</v>
+      </c>
+      <c r="E29">
+        <v>575</v>
+      </c>
+      <c r="F29">
+        <v>295</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <v>3</v>
+      </c>
+      <c r="I29" s="1">
+        <v>3.8657407407407404E-2</v>
+      </c>
+      <c r="J29">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30">
+        <v>4</v>
+      </c>
+      <c r="C30">
+        <v>1215</v>
+      </c>
+      <c r="D30">
+        <v>965</v>
+      </c>
+      <c r="E30">
+        <v>735</v>
+      </c>
+      <c r="F30">
+        <v>375</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+      <c r="H30">
+        <v>4</v>
+      </c>
+      <c r="I30" s="1">
+        <v>4.8263888888888891E-2</v>
+      </c>
+      <c r="J30">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>55</v>
+      </c>
+      <c r="B31">
+        <v>5</v>
+      </c>
+      <c r="C31">
+        <v>1555</v>
+      </c>
+      <c r="D31">
+        <v>1235</v>
+      </c>
+      <c r="E31">
+        <v>940</v>
+      </c>
+      <c r="F31">
+        <v>485</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="H31">
+        <v>5</v>
+      </c>
+      <c r="I31" s="1">
+        <v>5.949074074074074E-2</v>
+      </c>
+      <c r="J31">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32">
+        <v>6</v>
+      </c>
+      <c r="C32">
+        <v>1995</v>
+      </c>
+      <c r="D32">
+        <v>1580</v>
+      </c>
+      <c r="E32">
+        <v>1205</v>
+      </c>
+      <c r="F32">
+        <v>620</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32">
+        <v>6</v>
+      </c>
+      <c r="I32" s="1">
+        <v>7.2453703703703701E-2</v>
+      </c>
+      <c r="J32">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>55</v>
+      </c>
+      <c r="B33">
+        <v>7</v>
+      </c>
+      <c r="C33">
+        <v>2550</v>
+      </c>
+      <c r="D33">
+        <v>2025</v>
+      </c>
+      <c r="E33">
+        <v>1540</v>
+      </c>
+      <c r="F33">
+        <v>790</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+      <c r="H33">
+        <v>7</v>
+      </c>
+      <c r="I33" s="1">
+        <v>8.7615740740740744E-2</v>
+      </c>
+      <c r="J33">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>55</v>
+      </c>
+      <c r="B34">
+        <v>8</v>
+      </c>
+      <c r="C34">
+        <v>3265</v>
+      </c>
+      <c r="D34">
+        <v>2590</v>
+      </c>
+      <c r="E34">
+        <v>1970</v>
+      </c>
+      <c r="F34">
+        <v>1015</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+      <c r="H34">
+        <v>9</v>
+      </c>
+      <c r="I34" s="1">
+        <v>0.1050925925925926</v>
+      </c>
+      <c r="J34">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>55</v>
+      </c>
+      <c r="B35">
+        <v>9</v>
+      </c>
+      <c r="C35">
+        <v>4180</v>
+      </c>
+      <c r="D35">
+        <v>3315</v>
+      </c>
+      <c r="E35">
+        <v>2520</v>
+      </c>
+      <c r="F35">
+        <v>1295</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+      <c r="H35">
+        <v>10</v>
+      </c>
+      <c r="I35" s="1">
+        <v>0.12534722222222222</v>
+      </c>
+      <c r="J35">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>55</v>
+      </c>
+      <c r="B36">
+        <v>10</v>
+      </c>
+      <c r="C36">
+        <v>5350</v>
+      </c>
+      <c r="D36">
+        <v>4245</v>
+      </c>
+      <c r="E36">
+        <v>3230</v>
+      </c>
+      <c r="F36">
+        <v>1660</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+      <c r="H36">
+        <v>12</v>
+      </c>
+      <c r="I36" s="1">
+        <v>0.14884259259259258</v>
+      </c>
+      <c r="J36">
+        <v>200</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added multiple new building classes
</commit_message>
<xml_diff>
--- a/Raw_Building_Data.xlsx
+++ b/Raw_Building_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pyeac\Desktop\Travian Sim V2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7933862-66C7-4ACC-B34E-DC61D7B67FBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BB2CCB3-7E5F-4C1B-8868-6FBC7E6C0506}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{D964349E-A6D7-42EF-9507-D8E4572606D0}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="60">
   <si>
     <t>Building</t>
   </si>
@@ -252,10 +252,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2864,13 +2865,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{559C895B-DEBC-4F15-AD65-1EAADE192C37}">
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:J136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.54296875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -2956,7 +2960,7 @@
         <v>2880</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -2988,7 +2992,7 @@
         <v>5185</v>
       </c>
       <c r="G4">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="H4">
         <v>2</v>
@@ -3020,7 +3024,7 @@
         <v>9330</v>
       </c>
       <c r="G5">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="H5">
         <v>2</v>
@@ -3052,7 +3056,7 @@
         <v>16795</v>
       </c>
       <c r="G6">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="H6">
         <v>2</v>
@@ -3116,7 +3120,7 @@
         <v>90</v>
       </c>
       <c r="G8">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H8">
         <v>1</v>
@@ -3148,7 +3152,7 @@
         <v>160</v>
       </c>
       <c r="G9">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H9">
         <v>2</v>
@@ -3180,7 +3184,7 @@
         <v>290</v>
       </c>
       <c r="G10">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="H10">
         <v>2</v>
@@ -3212,7 +3216,7 @@
         <v>525</v>
       </c>
       <c r="G11">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="H11">
         <v>2</v>
@@ -3276,7 +3280,7 @@
         <v>2230</v>
       </c>
       <c r="G13">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -3308,7 +3312,7 @@
         <v>4020</v>
       </c>
       <c r="G14">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H14">
         <v>2</v>
@@ -3340,7 +3344,7 @@
         <v>7230</v>
       </c>
       <c r="G15">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="H15">
         <v>2</v>
@@ -3372,7 +3376,7 @@
         <v>13015</v>
       </c>
       <c r="G16">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="H16">
         <v>2</v>
@@ -3436,7 +3440,7 @@
         <v>215</v>
       </c>
       <c r="G18">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="H18">
         <v>1</v>
@@ -3468,7 +3472,7 @@
         <v>390</v>
       </c>
       <c r="G19">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="H19">
         <v>2</v>
@@ -3500,7 +3504,7 @@
         <v>700</v>
       </c>
       <c r="G20">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="H20">
         <v>2</v>
@@ -3532,7 +3536,7 @@
         <v>1260</v>
       </c>
       <c r="G21">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="H21">
         <v>2</v>
@@ -3596,7 +3600,7 @@
         <v>160</v>
       </c>
       <c r="G23">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H23">
         <v>1</v>
@@ -3628,7 +3632,7 @@
         <v>290</v>
       </c>
       <c r="G24">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="H24">
         <v>2</v>
@@ -3660,7 +3664,7 @@
         <v>525</v>
       </c>
       <c r="G25">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="H25">
         <v>2</v>
@@ -3692,7 +3696,7 @@
         <v>945</v>
       </c>
       <c r="G26">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="H26">
         <v>2</v>
@@ -3756,7 +3760,7 @@
         <v>230</v>
       </c>
       <c r="G28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H28">
         <v>3</v>
@@ -3788,7 +3792,7 @@
         <v>295</v>
       </c>
       <c r="G29">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H29">
         <v>3</v>
@@ -3820,7 +3824,7 @@
         <v>375</v>
       </c>
       <c r="G30">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H30">
         <v>4</v>
@@ -3852,7 +3856,7 @@
         <v>485</v>
       </c>
       <c r="G31">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H31">
         <v>5</v>
@@ -3884,7 +3888,7 @@
         <v>620</v>
       </c>
       <c r="G32">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H32">
         <v>6</v>
@@ -3916,7 +3920,7 @@
         <v>790</v>
       </c>
       <c r="G33">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="H33">
         <v>7</v>
@@ -3948,7 +3952,7 @@
         <v>1015</v>
       </c>
       <c r="G34">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="H34">
         <v>9</v>
@@ -3980,7 +3984,7 @@
         <v>1295</v>
       </c>
       <c r="G35">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="H35">
         <v>10</v>
@@ -4012,7 +4016,7 @@
         <v>1660</v>
       </c>
       <c r="G36">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="H36">
         <v>12</v>
@@ -4022,6 +4026,3206 @@
       </c>
       <c r="J36">
         <v>200</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>55</v>
+      </c>
+      <c r="B37">
+        <v>11</v>
+      </c>
+      <c r="C37">
+        <v>6845</v>
+      </c>
+      <c r="D37">
+        <v>5430</v>
+      </c>
+      <c r="E37">
+        <v>4130</v>
+      </c>
+      <c r="F37">
+        <v>2125</v>
+      </c>
+      <c r="G37">
+        <v>12</v>
+      </c>
+      <c r="H37">
+        <v>15</v>
+      </c>
+      <c r="I37" s="1">
+        <v>0.1761574074074074</v>
+      </c>
+      <c r="J37">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>55</v>
+      </c>
+      <c r="B38">
+        <v>12</v>
+      </c>
+      <c r="C38">
+        <v>8765</v>
+      </c>
+      <c r="D38">
+        <v>6950</v>
+      </c>
+      <c r="E38">
+        <v>5290</v>
+      </c>
+      <c r="F38">
+        <v>2720</v>
+      </c>
+      <c r="G38">
+        <v>14</v>
+      </c>
+      <c r="H38">
+        <v>18</v>
+      </c>
+      <c r="I38" s="1">
+        <v>0.20775462962962962</v>
+      </c>
+      <c r="J38">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>55</v>
+      </c>
+      <c r="B39">
+        <v>13</v>
+      </c>
+      <c r="C39">
+        <v>11220</v>
+      </c>
+      <c r="D39">
+        <v>8900</v>
+      </c>
+      <c r="E39">
+        <v>6770</v>
+      </c>
+      <c r="F39">
+        <v>3480</v>
+      </c>
+      <c r="G39">
+        <v>16</v>
+      </c>
+      <c r="H39">
+        <v>21</v>
+      </c>
+      <c r="I39" s="1">
+        <v>0.24456018518518519</v>
+      </c>
+      <c r="J39">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>55</v>
+      </c>
+      <c r="B40">
+        <v>14</v>
+      </c>
+      <c r="C40">
+        <v>14360</v>
+      </c>
+      <c r="D40">
+        <v>11390</v>
+      </c>
+      <c r="E40">
+        <v>8665</v>
+      </c>
+      <c r="F40">
+        <v>4455</v>
+      </c>
+      <c r="G40">
+        <v>18</v>
+      </c>
+      <c r="H40">
+        <v>26</v>
+      </c>
+      <c r="I40" s="1">
+        <v>0.28715277777777776</v>
+      </c>
+      <c r="J40">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>55</v>
+      </c>
+      <c r="B41">
+        <v>15</v>
+      </c>
+      <c r="C41">
+        <v>18380</v>
+      </c>
+      <c r="D41">
+        <v>14580</v>
+      </c>
+      <c r="E41">
+        <v>11090</v>
+      </c>
+      <c r="F41">
+        <v>5705</v>
+      </c>
+      <c r="G41">
+        <v>20</v>
+      </c>
+      <c r="H41">
+        <v>31</v>
+      </c>
+      <c r="I41" s="1">
+        <v>0.33657407407407408</v>
+      </c>
+      <c r="J41">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>55</v>
+      </c>
+      <c r="B42">
+        <v>16</v>
+      </c>
+      <c r="C42">
+        <v>23530</v>
+      </c>
+      <c r="D42">
+        <v>18660</v>
+      </c>
+      <c r="E42">
+        <v>14200</v>
+      </c>
+      <c r="F42">
+        <v>7300</v>
+      </c>
+      <c r="G42">
+        <v>22</v>
+      </c>
+      <c r="H42">
+        <v>37</v>
+      </c>
+      <c r="I42" s="1">
+        <v>0.39386574074074077</v>
+      </c>
+      <c r="J42">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>55</v>
+      </c>
+      <c r="B43">
+        <v>17</v>
+      </c>
+      <c r="C43">
+        <v>30115</v>
+      </c>
+      <c r="D43">
+        <v>23885</v>
+      </c>
+      <c r="E43">
+        <v>18175</v>
+      </c>
+      <c r="F43">
+        <v>9345</v>
+      </c>
+      <c r="G43">
+        <v>24</v>
+      </c>
+      <c r="H43">
+        <v>44</v>
+      </c>
+      <c r="I43" s="1">
+        <v>0.46030092592592592</v>
+      </c>
+      <c r="J43">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>55</v>
+      </c>
+      <c r="B44">
+        <v>18</v>
+      </c>
+      <c r="C44">
+        <v>38550</v>
+      </c>
+      <c r="D44">
+        <v>30570</v>
+      </c>
+      <c r="E44">
+        <v>23260</v>
+      </c>
+      <c r="F44">
+        <v>11965</v>
+      </c>
+      <c r="G44">
+        <v>26</v>
+      </c>
+      <c r="H44">
+        <v>53</v>
+      </c>
+      <c r="I44" s="1">
+        <v>0.53749999999999998</v>
+      </c>
+      <c r="J44">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>55</v>
+      </c>
+      <c r="B45">
+        <v>19</v>
+      </c>
+      <c r="C45">
+        <v>49340</v>
+      </c>
+      <c r="D45">
+        <v>39130</v>
+      </c>
+      <c r="E45">
+        <v>29775</v>
+      </c>
+      <c r="F45">
+        <v>15315</v>
+      </c>
+      <c r="G45">
+        <v>28</v>
+      </c>
+      <c r="H45">
+        <v>64</v>
+      </c>
+      <c r="I45" s="1">
+        <v>0.6269675925925926</v>
+      </c>
+      <c r="J45">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>55</v>
+      </c>
+      <c r="B46">
+        <v>20</v>
+      </c>
+      <c r="C46">
+        <v>63155</v>
+      </c>
+      <c r="D46">
+        <v>50090</v>
+      </c>
+      <c r="E46">
+        <v>38110</v>
+      </c>
+      <c r="F46">
+        <v>19600</v>
+      </c>
+      <c r="G46">
+        <v>30</v>
+      </c>
+      <c r="H46">
+        <v>77</v>
+      </c>
+      <c r="I46" s="1">
+        <v>0.73067129629629635</v>
+      </c>
+      <c r="J46">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>58</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47">
+        <v>2880</v>
+      </c>
+      <c r="D47">
+        <v>2740</v>
+      </c>
+      <c r="E47">
+        <v>2580</v>
+      </c>
+      <c r="F47">
+        <v>990</v>
+      </c>
+      <c r="G47">
+        <v>4</v>
+      </c>
+      <c r="H47">
+        <v>7</v>
+      </c>
+      <c r="I47" s="1">
+        <v>9.2592592592592587E-2</v>
+      </c>
+      <c r="J47" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>58</v>
+      </c>
+      <c r="B48">
+        <v>2</v>
+      </c>
+      <c r="C48">
+        <v>3630</v>
+      </c>
+      <c r="D48">
+        <v>3450</v>
+      </c>
+      <c r="E48">
+        <v>3250</v>
+      </c>
+      <c r="F48">
+        <v>1245</v>
+      </c>
+      <c r="G48">
+        <v>6</v>
+      </c>
+      <c r="H48">
+        <v>9</v>
+      </c>
+      <c r="I48" s="1">
+        <v>0.11087962962962963</v>
+      </c>
+      <c r="J48" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>58</v>
+      </c>
+      <c r="B49">
+        <v>3</v>
+      </c>
+      <c r="C49">
+        <v>4570</v>
+      </c>
+      <c r="D49">
+        <v>4350</v>
+      </c>
+      <c r="E49">
+        <v>4095</v>
+      </c>
+      <c r="F49">
+        <v>1570</v>
+      </c>
+      <c r="G49">
+        <v>8</v>
+      </c>
+      <c r="H49">
+        <v>10</v>
+      </c>
+      <c r="I49" s="1">
+        <v>0.1320601851851852</v>
+      </c>
+      <c r="J49" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>58</v>
+      </c>
+      <c r="B50">
+        <v>4</v>
+      </c>
+      <c r="C50">
+        <v>5760</v>
+      </c>
+      <c r="D50">
+        <v>5480</v>
+      </c>
+      <c r="E50">
+        <v>5160</v>
+      </c>
+      <c r="F50">
+        <v>1980</v>
+      </c>
+      <c r="G50">
+        <v>10</v>
+      </c>
+      <c r="H50">
+        <v>12</v>
+      </c>
+      <c r="I50" s="1">
+        <v>0.15671296296296297</v>
+      </c>
+      <c r="J50" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>58</v>
+      </c>
+      <c r="B51">
+        <v>5</v>
+      </c>
+      <c r="C51">
+        <v>7260</v>
+      </c>
+      <c r="D51">
+        <v>6905</v>
+      </c>
+      <c r="E51">
+        <v>6505</v>
+      </c>
+      <c r="F51">
+        <v>2495</v>
+      </c>
+      <c r="G51">
+        <v>12</v>
+      </c>
+      <c r="H51">
+        <v>15</v>
+      </c>
+      <c r="I51" s="1">
+        <v>0.18530092592592592</v>
+      </c>
+      <c r="J51" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>58</v>
+      </c>
+      <c r="B52">
+        <v>6</v>
+      </c>
+      <c r="C52">
+        <v>9145</v>
+      </c>
+      <c r="D52">
+        <v>8700</v>
+      </c>
+      <c r="E52">
+        <v>8195</v>
+      </c>
+      <c r="F52">
+        <v>3145</v>
+      </c>
+      <c r="G52">
+        <v>15</v>
+      </c>
+      <c r="H52">
+        <v>18</v>
+      </c>
+      <c r="I52" s="1">
+        <v>0.21840277777777778</v>
+      </c>
+      <c r="J52" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>58</v>
+      </c>
+      <c r="B53">
+        <v>7</v>
+      </c>
+      <c r="C53">
+        <v>11525</v>
+      </c>
+      <c r="D53">
+        <v>10965</v>
+      </c>
+      <c r="E53">
+        <v>10325</v>
+      </c>
+      <c r="F53">
+        <v>3960</v>
+      </c>
+      <c r="G53">
+        <v>18</v>
+      </c>
+      <c r="H53">
+        <v>21</v>
+      </c>
+      <c r="I53" s="1">
+        <v>0.25671296296296298</v>
+      </c>
+      <c r="J53" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>58</v>
+      </c>
+      <c r="B54">
+        <v>8</v>
+      </c>
+      <c r="C54">
+        <v>14520</v>
+      </c>
+      <c r="D54">
+        <v>13815</v>
+      </c>
+      <c r="E54">
+        <v>13010</v>
+      </c>
+      <c r="F54">
+        <v>4990</v>
+      </c>
+      <c r="G54">
+        <v>21</v>
+      </c>
+      <c r="H54">
+        <v>26</v>
+      </c>
+      <c r="I54" s="1">
+        <v>0.30127314814814815</v>
+      </c>
+      <c r="J54" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>58</v>
+      </c>
+      <c r="B55">
+        <v>9</v>
+      </c>
+      <c r="C55">
+        <v>18295</v>
+      </c>
+      <c r="D55">
+        <v>17405</v>
+      </c>
+      <c r="E55">
+        <v>16390</v>
+      </c>
+      <c r="F55">
+        <v>6290</v>
+      </c>
+      <c r="G55">
+        <v>24</v>
+      </c>
+      <c r="H55">
+        <v>31</v>
+      </c>
+      <c r="I55" s="1">
+        <v>0.35300925925925924</v>
+      </c>
+      <c r="J55" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>58</v>
+      </c>
+      <c r="B56">
+        <v>10</v>
+      </c>
+      <c r="C56">
+        <v>23055</v>
+      </c>
+      <c r="D56">
+        <v>21930</v>
+      </c>
+      <c r="E56">
+        <v>20650</v>
+      </c>
+      <c r="F56">
+        <v>7925</v>
+      </c>
+      <c r="G56">
+        <v>27</v>
+      </c>
+      <c r="H56">
+        <v>37</v>
+      </c>
+      <c r="I56" s="1">
+        <v>0.41296296296296298</v>
+      </c>
+      <c r="J56" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>58</v>
+      </c>
+      <c r="B57">
+        <v>11</v>
+      </c>
+      <c r="C57">
+        <v>29045</v>
+      </c>
+      <c r="D57">
+        <v>27635</v>
+      </c>
+      <c r="E57">
+        <v>26020</v>
+      </c>
+      <c r="F57">
+        <v>9985</v>
+      </c>
+      <c r="G57">
+        <v>30</v>
+      </c>
+      <c r="H57">
+        <v>45</v>
+      </c>
+      <c r="I57" s="1">
+        <v>0.48252314814814817</v>
+      </c>
+      <c r="J57" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>58</v>
+      </c>
+      <c r="B58">
+        <v>12</v>
+      </c>
+      <c r="C58">
+        <v>36600</v>
+      </c>
+      <c r="D58">
+        <v>34820</v>
+      </c>
+      <c r="E58">
+        <v>32785</v>
+      </c>
+      <c r="F58">
+        <v>12580</v>
+      </c>
+      <c r="G58">
+        <v>33</v>
+      </c>
+      <c r="H58">
+        <v>53</v>
+      </c>
+      <c r="I58" s="1">
+        <v>0.56319444444444444</v>
+      </c>
+      <c r="J58" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>58</v>
+      </c>
+      <c r="B59">
+        <v>13</v>
+      </c>
+      <c r="C59">
+        <v>46115</v>
+      </c>
+      <c r="D59">
+        <v>43875</v>
+      </c>
+      <c r="E59">
+        <v>41310</v>
+      </c>
+      <c r="F59">
+        <v>15850</v>
+      </c>
+      <c r="G59">
+        <v>36</v>
+      </c>
+      <c r="H59">
+        <v>64</v>
+      </c>
+      <c r="I59" s="1">
+        <v>0.656712962962963</v>
+      </c>
+      <c r="J59" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>58</v>
+      </c>
+      <c r="B60">
+        <v>14</v>
+      </c>
+      <c r="C60">
+        <v>58105</v>
+      </c>
+      <c r="D60">
+        <v>55280</v>
+      </c>
+      <c r="E60">
+        <v>52050</v>
+      </c>
+      <c r="F60">
+        <v>19975</v>
+      </c>
+      <c r="G60">
+        <v>39</v>
+      </c>
+      <c r="H60">
+        <v>77</v>
+      </c>
+      <c r="I60" s="1">
+        <v>0.76527777777777772</v>
+      </c>
+      <c r="J60" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>58</v>
+      </c>
+      <c r="B61">
+        <v>15</v>
+      </c>
+      <c r="C61">
+        <v>73210</v>
+      </c>
+      <c r="D61">
+        <v>69655</v>
+      </c>
+      <c r="E61">
+        <v>65585</v>
+      </c>
+      <c r="F61">
+        <v>25165</v>
+      </c>
+      <c r="G61">
+        <v>42</v>
+      </c>
+      <c r="H61">
+        <v>92</v>
+      </c>
+      <c r="I61" s="1">
+        <v>0.89120370370370372</v>
+      </c>
+      <c r="J61" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>58</v>
+      </c>
+      <c r="B62">
+        <v>16</v>
+      </c>
+      <c r="C62">
+        <v>92245</v>
+      </c>
+      <c r="D62">
+        <v>87760</v>
+      </c>
+      <c r="E62">
+        <v>82640</v>
+      </c>
+      <c r="F62">
+        <v>31710</v>
+      </c>
+      <c r="G62">
+        <v>46</v>
+      </c>
+      <c r="H62">
+        <v>111</v>
+      </c>
+      <c r="I62" s="3">
+        <v>1.0372685185185184</v>
+      </c>
+      <c r="J62" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>58</v>
+      </c>
+      <c r="B63">
+        <v>17</v>
+      </c>
+      <c r="C63">
+        <v>116230</v>
+      </c>
+      <c r="D63">
+        <v>110580</v>
+      </c>
+      <c r="E63">
+        <v>104125</v>
+      </c>
+      <c r="F63">
+        <v>39955</v>
+      </c>
+      <c r="G63">
+        <v>50</v>
+      </c>
+      <c r="H63">
+        <v>133</v>
+      </c>
+      <c r="I63" s="3">
+        <v>1.2067129629629629</v>
+      </c>
+      <c r="J63" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>58</v>
+      </c>
+      <c r="B64">
+        <v>18</v>
+      </c>
+      <c r="C64">
+        <v>146450</v>
+      </c>
+      <c r="D64">
+        <v>139330</v>
+      </c>
+      <c r="E64">
+        <v>131195</v>
+      </c>
+      <c r="F64">
+        <v>50340</v>
+      </c>
+      <c r="G64">
+        <v>54</v>
+      </c>
+      <c r="H64">
+        <v>160</v>
+      </c>
+      <c r="I64" s="3">
+        <v>1.4032407407407408</v>
+      </c>
+      <c r="J64" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>58</v>
+      </c>
+      <c r="B65">
+        <v>19</v>
+      </c>
+      <c r="C65">
+        <v>184530</v>
+      </c>
+      <c r="D65">
+        <v>175560</v>
+      </c>
+      <c r="E65">
+        <v>165305</v>
+      </c>
+      <c r="F65">
+        <v>63430</v>
+      </c>
+      <c r="G65">
+        <v>58</v>
+      </c>
+      <c r="H65">
+        <v>192</v>
+      </c>
+      <c r="I65" s="3">
+        <v>1.6312500000000001</v>
+      </c>
+      <c r="J65" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>58</v>
+      </c>
+      <c r="B66">
+        <v>20</v>
+      </c>
+      <c r="C66">
+        <v>232505</v>
+      </c>
+      <c r="D66">
+        <v>221205</v>
+      </c>
+      <c r="E66">
+        <v>208285</v>
+      </c>
+      <c r="F66">
+        <v>79925</v>
+      </c>
+      <c r="G66">
+        <v>62</v>
+      </c>
+      <c r="H66">
+        <v>230</v>
+      </c>
+      <c r="I66" s="3">
+        <v>1.8957175925925926</v>
+      </c>
+      <c r="J66" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>56</v>
+      </c>
+      <c r="B67">
+        <v>1</v>
+      </c>
+      <c r="C67">
+        <v>1250</v>
+      </c>
+      <c r="D67">
+        <v>1110</v>
+      </c>
+      <c r="E67">
+        <v>1260</v>
+      </c>
+      <c r="F67">
+        <v>600</v>
+      </c>
+      <c r="G67">
+        <v>4</v>
+      </c>
+      <c r="H67">
+        <v>6</v>
+      </c>
+      <c r="I67" s="1">
+        <v>0.14467592592592593</v>
+      </c>
+      <c r="J67" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>56</v>
+      </c>
+      <c r="B68">
+        <v>2</v>
+      </c>
+      <c r="C68">
+        <v>1600</v>
+      </c>
+      <c r="D68">
+        <v>1420</v>
+      </c>
+      <c r="E68">
+        <v>1615</v>
+      </c>
+      <c r="F68">
+        <v>770</v>
+      </c>
+      <c r="G68">
+        <v>6</v>
+      </c>
+      <c r="H68">
+        <v>7</v>
+      </c>
+      <c r="I68" s="1">
+        <v>0.17129629629629631</v>
+      </c>
+      <c r="J68" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>56</v>
+      </c>
+      <c r="B69">
+        <v>3</v>
+      </c>
+      <c r="C69">
+        <v>2050</v>
+      </c>
+      <c r="D69">
+        <v>1820</v>
+      </c>
+      <c r="E69">
+        <v>2065</v>
+      </c>
+      <c r="F69">
+        <v>985</v>
+      </c>
+      <c r="G69">
+        <v>8</v>
+      </c>
+      <c r="H69">
+        <v>9</v>
+      </c>
+      <c r="I69" s="1">
+        <v>0.20219907407407409</v>
+      </c>
+      <c r="J69" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>56</v>
+      </c>
+      <c r="B70">
+        <v>4</v>
+      </c>
+      <c r="C70">
+        <v>2620</v>
+      </c>
+      <c r="D70">
+        <v>2330</v>
+      </c>
+      <c r="E70">
+        <v>2640</v>
+      </c>
+      <c r="F70">
+        <v>1260</v>
+      </c>
+      <c r="G70">
+        <v>10</v>
+      </c>
+      <c r="H70">
+        <v>10</v>
+      </c>
+      <c r="I70" s="1">
+        <v>0.23796296296296296</v>
+      </c>
+      <c r="J70" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>56</v>
+      </c>
+      <c r="B71">
+        <v>5</v>
+      </c>
+      <c r="C71">
+        <v>3355</v>
+      </c>
+      <c r="D71">
+        <v>2980</v>
+      </c>
+      <c r="E71">
+        <v>3380</v>
+      </c>
+      <c r="F71">
+        <v>1610</v>
+      </c>
+      <c r="G71">
+        <v>12</v>
+      </c>
+      <c r="H71">
+        <v>12</v>
+      </c>
+      <c r="I71" s="1">
+        <v>0.2795138888888889</v>
+      </c>
+      <c r="J71" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>56</v>
+      </c>
+      <c r="B72">
+        <v>6</v>
+      </c>
+      <c r="C72">
+        <v>4295</v>
+      </c>
+      <c r="D72">
+        <v>3815</v>
+      </c>
+      <c r="E72">
+        <v>4330</v>
+      </c>
+      <c r="F72">
+        <v>2060</v>
+      </c>
+      <c r="G72">
+        <v>15</v>
+      </c>
+      <c r="H72">
+        <v>15</v>
+      </c>
+      <c r="I72" s="1">
+        <v>0.32777777777777778</v>
+      </c>
+      <c r="J72" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>56</v>
+      </c>
+      <c r="B73">
+        <v>7</v>
+      </c>
+      <c r="C73">
+        <v>5500</v>
+      </c>
+      <c r="D73">
+        <v>4880</v>
+      </c>
+      <c r="E73">
+        <v>5540</v>
+      </c>
+      <c r="F73">
+        <v>2640</v>
+      </c>
+      <c r="G73">
+        <v>18</v>
+      </c>
+      <c r="H73">
+        <v>18</v>
+      </c>
+      <c r="I73" s="1">
+        <v>0.38368055555555558</v>
+      </c>
+      <c r="J73" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>56</v>
+      </c>
+      <c r="B74">
+        <v>8</v>
+      </c>
+      <c r="C74">
+        <v>7035</v>
+      </c>
+      <c r="D74">
+        <v>6250</v>
+      </c>
+      <c r="E74">
+        <v>7095</v>
+      </c>
+      <c r="F74">
+        <v>3380</v>
+      </c>
+      <c r="G74">
+        <v>21</v>
+      </c>
+      <c r="H74">
+        <v>21</v>
+      </c>
+      <c r="I74" s="1">
+        <v>0.44849537037037035</v>
+      </c>
+      <c r="J74" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>56</v>
+      </c>
+      <c r="B75">
+        <v>9</v>
+      </c>
+      <c r="C75">
+        <v>9005</v>
+      </c>
+      <c r="D75">
+        <v>8000</v>
+      </c>
+      <c r="E75">
+        <v>9080</v>
+      </c>
+      <c r="F75">
+        <v>4325</v>
+      </c>
+      <c r="G75">
+        <v>24</v>
+      </c>
+      <c r="H75">
+        <v>26</v>
+      </c>
+      <c r="I75" s="1">
+        <v>0.52372685185185186</v>
+      </c>
+      <c r="J75" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>56</v>
+      </c>
+      <c r="B76">
+        <v>10</v>
+      </c>
+      <c r="C76">
+        <v>11530</v>
+      </c>
+      <c r="D76">
+        <v>10240</v>
+      </c>
+      <c r="E76">
+        <v>11620</v>
+      </c>
+      <c r="F76">
+        <v>5535</v>
+      </c>
+      <c r="G76">
+        <v>27</v>
+      </c>
+      <c r="H76">
+        <v>31</v>
+      </c>
+      <c r="I76" s="1">
+        <v>0.61099537037037033</v>
+      </c>
+      <c r="J76" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>56</v>
+      </c>
+      <c r="B77">
+        <v>11</v>
+      </c>
+      <c r="C77">
+        <v>14755</v>
+      </c>
+      <c r="D77">
+        <v>13105</v>
+      </c>
+      <c r="E77">
+        <v>14875</v>
+      </c>
+      <c r="F77">
+        <v>7085</v>
+      </c>
+      <c r="G77">
+        <v>30</v>
+      </c>
+      <c r="H77">
+        <v>37</v>
+      </c>
+      <c r="I77" s="1">
+        <v>0.71226851851851847</v>
+      </c>
+      <c r="J77" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>56</v>
+      </c>
+      <c r="B78">
+        <v>12</v>
+      </c>
+      <c r="C78">
+        <v>18890</v>
+      </c>
+      <c r="D78">
+        <v>16775</v>
+      </c>
+      <c r="E78">
+        <v>19040</v>
+      </c>
+      <c r="F78">
+        <v>9065</v>
+      </c>
+      <c r="G78">
+        <v>33</v>
+      </c>
+      <c r="H78">
+        <v>45</v>
+      </c>
+      <c r="I78" s="1">
+        <v>0.82974537037037033</v>
+      </c>
+      <c r="J78" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>56</v>
+      </c>
+      <c r="B79">
+        <v>13</v>
+      </c>
+      <c r="C79">
+        <v>24180</v>
+      </c>
+      <c r="D79">
+        <v>21470</v>
+      </c>
+      <c r="E79">
+        <v>24370</v>
+      </c>
+      <c r="F79">
+        <v>11605</v>
+      </c>
+      <c r="G79">
+        <v>36</v>
+      </c>
+      <c r="H79">
+        <v>53</v>
+      </c>
+      <c r="I79" s="1">
+        <v>0.96597222222222223</v>
+      </c>
+      <c r="J79" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>56</v>
+      </c>
+      <c r="B80">
+        <v>14</v>
+      </c>
+      <c r="C80">
+        <v>30950</v>
+      </c>
+      <c r="D80">
+        <v>27480</v>
+      </c>
+      <c r="E80">
+        <v>31195</v>
+      </c>
+      <c r="F80">
+        <v>14855</v>
+      </c>
+      <c r="G80">
+        <v>39</v>
+      </c>
+      <c r="H80">
+        <v>64</v>
+      </c>
+      <c r="I80" s="3">
+        <v>1.1239583333333334</v>
+      </c>
+      <c r="J80" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>56</v>
+      </c>
+      <c r="B81">
+        <v>15</v>
+      </c>
+      <c r="C81">
+        <v>39615</v>
+      </c>
+      <c r="D81">
+        <v>35175</v>
+      </c>
+      <c r="E81">
+        <v>39930</v>
+      </c>
+      <c r="F81">
+        <v>19015</v>
+      </c>
+      <c r="G81">
+        <v>42</v>
+      </c>
+      <c r="H81">
+        <v>77</v>
+      </c>
+      <c r="I81" s="3">
+        <v>1.3072916666666667</v>
+      </c>
+      <c r="J81" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>56</v>
+      </c>
+      <c r="B82">
+        <v>16</v>
+      </c>
+      <c r="C82">
+        <v>50705</v>
+      </c>
+      <c r="D82">
+        <v>45025</v>
+      </c>
+      <c r="E82">
+        <v>51110</v>
+      </c>
+      <c r="F82">
+        <v>24340</v>
+      </c>
+      <c r="G82">
+        <v>46</v>
+      </c>
+      <c r="H82">
+        <v>92</v>
+      </c>
+      <c r="I82" s="3">
+        <v>1.5199074074074075</v>
+      </c>
+      <c r="J82" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>56</v>
+      </c>
+      <c r="B83">
+        <v>17</v>
+      </c>
+      <c r="C83">
+        <v>64905</v>
+      </c>
+      <c r="D83">
+        <v>57635</v>
+      </c>
+      <c r="E83">
+        <v>65425</v>
+      </c>
+      <c r="F83">
+        <v>31155</v>
+      </c>
+      <c r="G83">
+        <v>50</v>
+      </c>
+      <c r="H83">
+        <v>111</v>
+      </c>
+      <c r="I83" s="3">
+        <v>1.766550925925926</v>
+      </c>
+      <c r="J83" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>56</v>
+      </c>
+      <c r="B84">
+        <v>18</v>
+      </c>
+      <c r="C84">
+        <v>83075</v>
+      </c>
+      <c r="D84">
+        <v>73770</v>
+      </c>
+      <c r="E84">
+        <v>83740</v>
+      </c>
+      <c r="F84">
+        <v>39875</v>
+      </c>
+      <c r="G84">
+        <v>54</v>
+      </c>
+      <c r="H84">
+        <v>133</v>
+      </c>
+      <c r="I84" s="3">
+        <v>2.0526620370370372</v>
+      </c>
+      <c r="J84" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>56</v>
+      </c>
+      <c r="B85">
+        <v>19</v>
+      </c>
+      <c r="C85">
+        <v>106340</v>
+      </c>
+      <c r="D85">
+        <v>94430</v>
+      </c>
+      <c r="E85">
+        <v>107190</v>
+      </c>
+      <c r="F85">
+        <v>51040</v>
+      </c>
+      <c r="G85">
+        <v>58</v>
+      </c>
+      <c r="H85">
+        <v>160</v>
+      </c>
+      <c r="I85" s="3">
+        <v>2.3844907407407407</v>
+      </c>
+      <c r="J85" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>56</v>
+      </c>
+      <c r="B86">
+        <v>20</v>
+      </c>
+      <c r="C86">
+        <v>136115</v>
+      </c>
+      <c r="D86">
+        <v>120870</v>
+      </c>
+      <c r="E86">
+        <v>137200</v>
+      </c>
+      <c r="F86">
+        <v>65335</v>
+      </c>
+      <c r="G86">
+        <v>62</v>
+      </c>
+      <c r="H86">
+        <v>192</v>
+      </c>
+      <c r="I86" s="3">
+        <v>2.7695601851851852</v>
+      </c>
+      <c r="J86" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>53</v>
+      </c>
+      <c r="B87">
+        <v>1</v>
+      </c>
+      <c r="C87">
+        <v>80</v>
+      </c>
+      <c r="D87">
+        <v>70</v>
+      </c>
+      <c r="E87">
+        <v>120</v>
+      </c>
+      <c r="F87">
+        <v>70</v>
+      </c>
+      <c r="G87">
+        <v>4</v>
+      </c>
+      <c r="H87">
+        <v>4</v>
+      </c>
+      <c r="I87" s="1">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="J87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>53</v>
+      </c>
+      <c r="B88">
+        <v>2</v>
+      </c>
+      <c r="C88">
+        <v>100</v>
+      </c>
+      <c r="D88">
+        <v>90</v>
+      </c>
+      <c r="E88">
+        <v>155</v>
+      </c>
+      <c r="F88">
+        <v>90</v>
+      </c>
+      <c r="G88">
+        <v>6</v>
+      </c>
+      <c r="H88">
+        <v>4</v>
+      </c>
+      <c r="I88" s="1">
+        <v>2.7662037037037037E-2</v>
+      </c>
+      <c r="J88">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>53</v>
+      </c>
+      <c r="B89">
+        <v>3</v>
+      </c>
+      <c r="C89">
+        <v>130</v>
+      </c>
+      <c r="D89">
+        <v>115</v>
+      </c>
+      <c r="E89">
+        <v>195</v>
+      </c>
+      <c r="F89">
+        <v>115</v>
+      </c>
+      <c r="G89">
+        <v>8</v>
+      </c>
+      <c r="H89">
+        <v>5</v>
+      </c>
+      <c r="I89" s="1">
+        <v>3.5532407407407408E-2</v>
+      </c>
+      <c r="J89">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>53</v>
+      </c>
+      <c r="B90">
+        <v>4</v>
+      </c>
+      <c r="C90">
+        <v>170</v>
+      </c>
+      <c r="D90">
+        <v>145</v>
+      </c>
+      <c r="E90">
+        <v>250</v>
+      </c>
+      <c r="F90">
+        <v>145</v>
+      </c>
+      <c r="G90">
+        <v>10</v>
+      </c>
+      <c r="H90">
+        <v>6</v>
+      </c>
+      <c r="I90" s="1">
+        <v>4.4675925925925924E-2</v>
+      </c>
+      <c r="J90">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>53</v>
+      </c>
+      <c r="B91">
+        <v>5</v>
+      </c>
+      <c r="C91">
+        <v>215</v>
+      </c>
+      <c r="D91">
+        <v>190</v>
+      </c>
+      <c r="E91">
+        <v>320</v>
+      </c>
+      <c r="F91">
+        <v>190</v>
+      </c>
+      <c r="G91">
+        <v>12</v>
+      </c>
+      <c r="H91">
+        <v>7</v>
+      </c>
+      <c r="I91" s="1">
+        <v>5.5324074074074074E-2</v>
+      </c>
+      <c r="J91">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>53</v>
+      </c>
+      <c r="B92">
+        <v>6</v>
+      </c>
+      <c r="C92">
+        <v>275</v>
+      </c>
+      <c r="D92">
+        <v>240</v>
+      </c>
+      <c r="E92">
+        <v>410</v>
+      </c>
+      <c r="F92">
+        <v>240</v>
+      </c>
+      <c r="G92">
+        <v>15</v>
+      </c>
+      <c r="H92">
+        <v>9</v>
+      </c>
+      <c r="I92" s="1">
+        <v>6.7592592592592593E-2</v>
+      </c>
+      <c r="J92">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>53</v>
+      </c>
+      <c r="B93">
+        <v>7</v>
+      </c>
+      <c r="C93">
+        <v>350</v>
+      </c>
+      <c r="D93">
+        <v>310</v>
+      </c>
+      <c r="E93">
+        <v>530</v>
+      </c>
+      <c r="F93">
+        <v>310</v>
+      </c>
+      <c r="G93">
+        <v>18</v>
+      </c>
+      <c r="H93">
+        <v>11</v>
+      </c>
+      <c r="I93" s="1">
+        <v>8.1944444444444445E-2</v>
+      </c>
+      <c r="J93">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>53</v>
+      </c>
+      <c r="B94">
+        <v>8</v>
+      </c>
+      <c r="C94">
+        <v>450</v>
+      </c>
+      <c r="D94">
+        <v>395</v>
+      </c>
+      <c r="E94">
+        <v>675</v>
+      </c>
+      <c r="F94">
+        <v>395</v>
+      </c>
+      <c r="G94">
+        <v>21</v>
+      </c>
+      <c r="H94">
+        <v>13</v>
+      </c>
+      <c r="I94" s="1">
+        <v>9.8495370370370372E-2</v>
+      </c>
+      <c r="J94">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>53</v>
+      </c>
+      <c r="B95">
+        <v>9</v>
+      </c>
+      <c r="C95">
+        <v>575</v>
+      </c>
+      <c r="D95">
+        <v>505</v>
+      </c>
+      <c r="E95">
+        <v>865</v>
+      </c>
+      <c r="F95">
+        <v>505</v>
+      </c>
+      <c r="G95">
+        <v>24</v>
+      </c>
+      <c r="H95">
+        <v>15</v>
+      </c>
+      <c r="I95" s="1">
+        <v>0.11770833333333333</v>
+      </c>
+      <c r="J95">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>53</v>
+      </c>
+      <c r="B96">
+        <v>10</v>
+      </c>
+      <c r="C96">
+        <v>740</v>
+      </c>
+      <c r="D96">
+        <v>645</v>
+      </c>
+      <c r="E96">
+        <v>1105</v>
+      </c>
+      <c r="F96">
+        <v>645</v>
+      </c>
+      <c r="G96">
+        <v>27</v>
+      </c>
+      <c r="H96">
+        <v>19</v>
+      </c>
+      <c r="I96" s="1">
+        <v>0.14004629629629631</v>
+      </c>
+      <c r="J96">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>53</v>
+      </c>
+      <c r="B97">
+        <v>11</v>
+      </c>
+      <c r="C97">
+        <v>945</v>
+      </c>
+      <c r="D97">
+        <v>825</v>
+      </c>
+      <c r="E97">
+        <v>1415</v>
+      </c>
+      <c r="F97">
+        <v>825</v>
+      </c>
+      <c r="G97">
+        <v>30</v>
+      </c>
+      <c r="H97">
+        <v>22</v>
+      </c>
+      <c r="I97" s="1">
+        <v>0.16597222222222222</v>
+      </c>
+      <c r="J97">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>53</v>
+      </c>
+      <c r="B98">
+        <v>12</v>
+      </c>
+      <c r="C98">
+        <v>1210</v>
+      </c>
+      <c r="D98">
+        <v>1060</v>
+      </c>
+      <c r="E98">
+        <v>1815</v>
+      </c>
+      <c r="F98">
+        <v>1060</v>
+      </c>
+      <c r="G98">
+        <v>33</v>
+      </c>
+      <c r="H98">
+        <v>27</v>
+      </c>
+      <c r="I98" s="1">
+        <v>0.19594907407407408</v>
+      </c>
+      <c r="J98">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>53</v>
+      </c>
+      <c r="B99">
+        <v>13</v>
+      </c>
+      <c r="C99">
+        <v>1545</v>
+      </c>
+      <c r="D99">
+        <v>1355</v>
+      </c>
+      <c r="E99">
+        <v>2320</v>
+      </c>
+      <c r="F99">
+        <v>1355</v>
+      </c>
+      <c r="G99">
+        <v>36</v>
+      </c>
+      <c r="H99">
+        <v>32</v>
+      </c>
+      <c r="I99" s="1">
+        <v>0.23078703703703704</v>
+      </c>
+      <c r="J99">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>53</v>
+      </c>
+      <c r="B100">
+        <v>14</v>
+      </c>
+      <c r="C100">
+        <v>1980</v>
+      </c>
+      <c r="D100">
+        <v>1735</v>
+      </c>
+      <c r="E100">
+        <v>2970</v>
+      </c>
+      <c r="F100">
+        <v>1735</v>
+      </c>
+      <c r="G100">
+        <v>39</v>
+      </c>
+      <c r="H100">
+        <v>39</v>
+      </c>
+      <c r="I100" s="1">
+        <v>0.27118055555555554</v>
+      </c>
+      <c r="J100">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
+        <v>53</v>
+      </c>
+      <c r="B101">
+        <v>15</v>
+      </c>
+      <c r="C101">
+        <v>2535</v>
+      </c>
+      <c r="D101">
+        <v>2220</v>
+      </c>
+      <c r="E101">
+        <v>3805</v>
+      </c>
+      <c r="F101">
+        <v>2220</v>
+      </c>
+      <c r="G101">
+        <v>42</v>
+      </c>
+      <c r="H101">
+        <v>46</v>
+      </c>
+      <c r="I101" s="1">
+        <v>0.31805555555555554</v>
+      </c>
+      <c r="J101">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
+        <v>53</v>
+      </c>
+      <c r="B102">
+        <v>16</v>
+      </c>
+      <c r="C102">
+        <v>3245</v>
+      </c>
+      <c r="D102">
+        <v>2840</v>
+      </c>
+      <c r="E102">
+        <v>4870</v>
+      </c>
+      <c r="F102">
+        <v>2840</v>
+      </c>
+      <c r="G102">
+        <v>46</v>
+      </c>
+      <c r="H102">
+        <v>55</v>
+      </c>
+      <c r="I102" s="1">
+        <v>0.37245370370370373</v>
+      </c>
+      <c r="J102">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
+        <v>53</v>
+      </c>
+      <c r="B103">
+        <v>17</v>
+      </c>
+      <c r="C103">
+        <v>4155</v>
+      </c>
+      <c r="D103">
+        <v>3635</v>
+      </c>
+      <c r="E103">
+        <v>6230</v>
+      </c>
+      <c r="F103">
+        <v>3635</v>
+      </c>
+      <c r="G103">
+        <v>50</v>
+      </c>
+      <c r="H103">
+        <v>67</v>
+      </c>
+      <c r="I103" s="1">
+        <v>0.43541666666666667</v>
+      </c>
+      <c r="J103">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
+        <v>53</v>
+      </c>
+      <c r="B104">
+        <v>18</v>
+      </c>
+      <c r="C104">
+        <v>5315</v>
+      </c>
+      <c r="D104">
+        <v>4650</v>
+      </c>
+      <c r="E104">
+        <v>7975</v>
+      </c>
+      <c r="F104">
+        <v>4650</v>
+      </c>
+      <c r="G104">
+        <v>54</v>
+      </c>
+      <c r="H104">
+        <v>80</v>
+      </c>
+      <c r="I104" s="1">
+        <v>0.50856481481481486</v>
+      </c>
+      <c r="J104">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
+        <v>53</v>
+      </c>
+      <c r="B105">
+        <v>19</v>
+      </c>
+      <c r="C105">
+        <v>6805</v>
+      </c>
+      <c r="D105">
+        <v>5955</v>
+      </c>
+      <c r="E105">
+        <v>10210</v>
+      </c>
+      <c r="F105">
+        <v>5955</v>
+      </c>
+      <c r="G105">
+        <v>58</v>
+      </c>
+      <c r="H105">
+        <v>96</v>
+      </c>
+      <c r="I105" s="1">
+        <v>0.59340277777777772</v>
+      </c>
+      <c r="J105">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
+        <v>53</v>
+      </c>
+      <c r="B106">
+        <v>20</v>
+      </c>
+      <c r="C106">
+        <v>8710</v>
+      </c>
+      <c r="D106">
+        <v>7620</v>
+      </c>
+      <c r="E106">
+        <v>13065</v>
+      </c>
+      <c r="F106">
+        <v>7620</v>
+      </c>
+      <c r="G106">
+        <v>62</v>
+      </c>
+      <c r="H106">
+        <v>115</v>
+      </c>
+      <c r="I106" s="1">
+        <v>0.6918981481481481</v>
+      </c>
+      <c r="J106">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
+        <v>51</v>
+      </c>
+      <c r="B107">
+        <v>1</v>
+      </c>
+      <c r="C107">
+        <v>180</v>
+      </c>
+      <c r="D107">
+        <v>130</v>
+      </c>
+      <c r="E107">
+        <v>150</v>
+      </c>
+      <c r="F107">
+        <v>80</v>
+      </c>
+      <c r="G107">
+        <v>3</v>
+      </c>
+      <c r="H107">
+        <v>5</v>
+      </c>
+      <c r="I107" s="1">
+        <v>2.3148148148148147E-2</v>
+      </c>
+      <c r="J107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
+        <v>51</v>
+      </c>
+      <c r="B108">
+        <v>2</v>
+      </c>
+      <c r="C108">
+        <v>230</v>
+      </c>
+      <c r="D108">
+        <v>165</v>
+      </c>
+      <c r="E108">
+        <v>190</v>
+      </c>
+      <c r="F108">
+        <v>100</v>
+      </c>
+      <c r="G108">
+        <v>5</v>
+      </c>
+      <c r="H108">
+        <v>6</v>
+      </c>
+      <c r="I108" s="1">
+        <v>3.0324074074074073E-2</v>
+      </c>
+      <c r="J108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
+        <v>51</v>
+      </c>
+      <c r="B109">
+        <v>3</v>
+      </c>
+      <c r="C109">
+        <v>295</v>
+      </c>
+      <c r="D109">
+        <v>215</v>
+      </c>
+      <c r="E109">
+        <v>245</v>
+      </c>
+      <c r="F109">
+        <v>130</v>
+      </c>
+      <c r="G109">
+        <v>7</v>
+      </c>
+      <c r="H109">
+        <v>7</v>
+      </c>
+      <c r="I109" s="1">
+        <v>3.8657407407407404E-2</v>
+      </c>
+      <c r="J109">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
+        <v>51</v>
+      </c>
+      <c r="B110">
+        <v>4</v>
+      </c>
+      <c r="C110">
+        <v>375</v>
+      </c>
+      <c r="D110">
+        <v>275</v>
+      </c>
+      <c r="E110">
+        <v>315</v>
+      </c>
+      <c r="F110">
+        <v>170</v>
+      </c>
+      <c r="G110">
+        <v>9</v>
+      </c>
+      <c r="H110">
+        <v>8</v>
+      </c>
+      <c r="I110" s="1">
+        <v>4.8263888888888891E-2</v>
+      </c>
+      <c r="J110">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
+        <v>51</v>
+      </c>
+      <c r="B111">
+        <v>5</v>
+      </c>
+      <c r="C111">
+        <v>485</v>
+      </c>
+      <c r="D111">
+        <v>350</v>
+      </c>
+      <c r="E111">
+        <v>405</v>
+      </c>
+      <c r="F111">
+        <v>215</v>
+      </c>
+      <c r="G111">
+        <v>11</v>
+      </c>
+      <c r="H111">
+        <v>10</v>
+      </c>
+      <c r="I111" s="1">
+        <v>5.949074074074074E-2</v>
+      </c>
+      <c r="J111">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
+        <v>51</v>
+      </c>
+      <c r="B112">
+        <v>6</v>
+      </c>
+      <c r="C112">
+        <v>620</v>
+      </c>
+      <c r="D112">
+        <v>445</v>
+      </c>
+      <c r="E112">
+        <v>515</v>
+      </c>
+      <c r="F112">
+        <v>275</v>
+      </c>
+      <c r="G112">
+        <v>13</v>
+      </c>
+      <c r="H112">
+        <v>12</v>
+      </c>
+      <c r="I112" s="1">
+        <v>7.2453703703703701E-2</v>
+      </c>
+      <c r="J112">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A113" t="s">
+        <v>51</v>
+      </c>
+      <c r="B113">
+        <v>7</v>
+      </c>
+      <c r="C113">
+        <v>790</v>
+      </c>
+      <c r="D113">
+        <v>570</v>
+      </c>
+      <c r="E113">
+        <v>660</v>
+      </c>
+      <c r="F113">
+        <v>350</v>
+      </c>
+      <c r="G113">
+        <v>15</v>
+      </c>
+      <c r="H113">
+        <v>14</v>
+      </c>
+      <c r="I113" s="1">
+        <v>8.7615740740740744E-2</v>
+      </c>
+      <c r="J113">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
+        <v>51</v>
+      </c>
+      <c r="B114">
+        <v>8</v>
+      </c>
+      <c r="C114">
+        <v>1015</v>
+      </c>
+      <c r="D114">
+        <v>730</v>
+      </c>
+      <c r="E114">
+        <v>845</v>
+      </c>
+      <c r="F114">
+        <v>450</v>
+      </c>
+      <c r="G114">
+        <v>17</v>
+      </c>
+      <c r="H114">
+        <v>17</v>
+      </c>
+      <c r="I114" s="1">
+        <v>0.1050925925925926</v>
+      </c>
+      <c r="J114">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A115" t="s">
+        <v>51</v>
+      </c>
+      <c r="B115">
+        <v>9</v>
+      </c>
+      <c r="C115">
+        <v>1295</v>
+      </c>
+      <c r="D115">
+        <v>935</v>
+      </c>
+      <c r="E115">
+        <v>1080</v>
+      </c>
+      <c r="F115">
+        <v>575</v>
+      </c>
+      <c r="G115">
+        <v>19</v>
+      </c>
+      <c r="H115">
+        <v>21</v>
+      </c>
+      <c r="I115" s="1">
+        <v>0.12534722222222222</v>
+      </c>
+      <c r="J115">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
+        <v>51</v>
+      </c>
+      <c r="B116">
+        <v>10</v>
+      </c>
+      <c r="C116">
+        <v>1660</v>
+      </c>
+      <c r="D116">
+        <v>1200</v>
+      </c>
+      <c r="E116">
+        <v>1385</v>
+      </c>
+      <c r="F116">
+        <v>740</v>
+      </c>
+      <c r="G116">
+        <v>21</v>
+      </c>
+      <c r="H116">
+        <v>25</v>
+      </c>
+      <c r="I116" s="1">
+        <v>0.14884259259259258</v>
+      </c>
+      <c r="J116">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
+        <v>51</v>
+      </c>
+      <c r="B117">
+        <v>11</v>
+      </c>
+      <c r="C117">
+        <v>2125</v>
+      </c>
+      <c r="D117">
+        <v>1535</v>
+      </c>
+      <c r="E117">
+        <v>1770</v>
+      </c>
+      <c r="F117">
+        <v>945</v>
+      </c>
+      <c r="G117">
+        <v>24</v>
+      </c>
+      <c r="H117">
+        <v>30</v>
+      </c>
+      <c r="I117" s="1">
+        <v>0.1761574074074074</v>
+      </c>
+      <c r="J117">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A118" t="s">
+        <v>51</v>
+      </c>
+      <c r="B118">
+        <v>12</v>
+      </c>
+      <c r="C118">
+        <v>2720</v>
+      </c>
+      <c r="D118">
+        <v>1965</v>
+      </c>
+      <c r="E118">
+        <v>2265</v>
+      </c>
+      <c r="F118">
+        <v>1210</v>
+      </c>
+      <c r="G118">
+        <v>27</v>
+      </c>
+      <c r="H118">
+        <v>36</v>
+      </c>
+      <c r="I118" s="1">
+        <v>0.20775462962962962</v>
+      </c>
+      <c r="J118">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
+        <v>51</v>
+      </c>
+      <c r="B119">
+        <v>13</v>
+      </c>
+      <c r="C119">
+        <v>3480</v>
+      </c>
+      <c r="D119">
+        <v>2515</v>
+      </c>
+      <c r="E119">
+        <v>2900</v>
+      </c>
+      <c r="F119">
+        <v>1545</v>
+      </c>
+      <c r="G119">
+        <v>30</v>
+      </c>
+      <c r="H119">
+        <v>43</v>
+      </c>
+      <c r="I119" s="1">
+        <v>0.24456018518518519</v>
+      </c>
+      <c r="J119">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A120" t="s">
+        <v>51</v>
+      </c>
+      <c r="B120">
+        <v>14</v>
+      </c>
+      <c r="C120">
+        <v>4455</v>
+      </c>
+      <c r="D120">
+        <v>3220</v>
+      </c>
+      <c r="E120">
+        <v>3715</v>
+      </c>
+      <c r="F120">
+        <v>1980</v>
+      </c>
+      <c r="G120">
+        <v>33</v>
+      </c>
+      <c r="H120">
+        <v>51</v>
+      </c>
+      <c r="I120" s="1">
+        <v>0.28715277777777776</v>
+      </c>
+      <c r="J120">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A121" t="s">
+        <v>51</v>
+      </c>
+      <c r="B121">
+        <v>15</v>
+      </c>
+      <c r="C121">
+        <v>5705</v>
+      </c>
+      <c r="D121">
+        <v>4120</v>
+      </c>
+      <c r="E121">
+        <v>4755</v>
+      </c>
+      <c r="F121">
+        <v>2535</v>
+      </c>
+      <c r="G121">
+        <v>36</v>
+      </c>
+      <c r="H121">
+        <v>62</v>
+      </c>
+      <c r="I121" s="1">
+        <v>0.33657407407407408</v>
+      </c>
+      <c r="J121">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A122" t="s">
+        <v>51</v>
+      </c>
+      <c r="B122">
+        <v>16</v>
+      </c>
+      <c r="C122">
+        <v>7300</v>
+      </c>
+      <c r="D122">
+        <v>5275</v>
+      </c>
+      <c r="E122">
+        <v>6085</v>
+      </c>
+      <c r="F122">
+        <v>3245</v>
+      </c>
+      <c r="G122">
+        <v>39</v>
+      </c>
+      <c r="H122">
+        <v>74</v>
+      </c>
+      <c r="I122" s="1">
+        <v>0.39386574074074077</v>
+      </c>
+      <c r="J122">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
+        <v>51</v>
+      </c>
+      <c r="B123">
+        <v>17</v>
+      </c>
+      <c r="C123">
+        <v>9345</v>
+      </c>
+      <c r="D123">
+        <v>6750</v>
+      </c>
+      <c r="E123">
+        <v>7790</v>
+      </c>
+      <c r="F123">
+        <v>4155</v>
+      </c>
+      <c r="G123">
+        <v>42</v>
+      </c>
+      <c r="H123">
+        <v>89</v>
+      </c>
+      <c r="I123" s="1">
+        <v>0.46030092592592592</v>
+      </c>
+      <c r="J123">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
+        <v>51</v>
+      </c>
+      <c r="B124">
+        <v>18</v>
+      </c>
+      <c r="C124">
+        <v>11965</v>
+      </c>
+      <c r="D124">
+        <v>8640</v>
+      </c>
+      <c r="E124">
+        <v>9970</v>
+      </c>
+      <c r="F124">
+        <v>5315</v>
+      </c>
+      <c r="G124">
+        <v>45</v>
+      </c>
+      <c r="H124">
+        <v>106</v>
+      </c>
+      <c r="I124" s="1">
+        <v>0.53749999999999998</v>
+      </c>
+      <c r="J124">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A125" t="s">
+        <v>51</v>
+      </c>
+      <c r="B125">
+        <v>19</v>
+      </c>
+      <c r="C125">
+        <v>15315</v>
+      </c>
+      <c r="D125">
+        <v>11060</v>
+      </c>
+      <c r="E125">
+        <v>12760</v>
+      </c>
+      <c r="F125">
+        <v>6805</v>
+      </c>
+      <c r="G125">
+        <v>48</v>
+      </c>
+      <c r="H125">
+        <v>128</v>
+      </c>
+      <c r="I125" s="1">
+        <v>0.6269675925925926</v>
+      </c>
+      <c r="J125">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A126" t="s">
+        <v>51</v>
+      </c>
+      <c r="B126">
+        <v>20</v>
+      </c>
+      <c r="C126">
+        <v>19600</v>
+      </c>
+      <c r="D126">
+        <v>14155</v>
+      </c>
+      <c r="E126">
+        <v>16335</v>
+      </c>
+      <c r="F126">
+        <v>8710</v>
+      </c>
+      <c r="G126">
+        <v>51</v>
+      </c>
+      <c r="H126">
+        <v>153</v>
+      </c>
+      <c r="I126" s="1">
+        <v>0.73067129629629635</v>
+      </c>
+      <c r="J126">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A127" t="s">
+        <v>50</v>
+      </c>
+      <c r="B127">
+        <v>1</v>
+      </c>
+      <c r="C127">
+        <v>40</v>
+      </c>
+      <c r="D127">
+        <v>50</v>
+      </c>
+      <c r="E127">
+        <v>30</v>
+      </c>
+      <c r="F127">
+        <v>10</v>
+      </c>
+      <c r="G127">
+        <v>0</v>
+      </c>
+      <c r="H127">
+        <v>1</v>
+      </c>
+      <c r="I127" s="1">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="J127">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A128" t="s">
+        <v>50</v>
+      </c>
+      <c r="B128">
+        <v>2</v>
+      </c>
+      <c r="C128">
+        <v>50</v>
+      </c>
+      <c r="D128">
+        <v>65</v>
+      </c>
+      <c r="E128">
+        <v>40</v>
+      </c>
+      <c r="F128">
+        <v>15</v>
+      </c>
+      <c r="G128">
+        <v>0</v>
+      </c>
+      <c r="H128">
+        <v>1</v>
+      </c>
+      <c r="I128" s="1">
+        <v>7.5231481481481477E-3</v>
+      </c>
+      <c r="J128">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A129" t="s">
+        <v>50</v>
+      </c>
+      <c r="B129">
+        <v>3</v>
+      </c>
+      <c r="C129">
+        <v>65</v>
+      </c>
+      <c r="D129">
+        <v>80</v>
+      </c>
+      <c r="E129">
+        <v>50</v>
+      </c>
+      <c r="F129">
+        <v>15</v>
+      </c>
+      <c r="G129">
+        <v>0</v>
+      </c>
+      <c r="H129">
+        <v>2</v>
+      </c>
+      <c r="I129" s="1">
+        <v>1.2152777777777778E-2</v>
+      </c>
+      <c r="J129">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A130" t="s">
+        <v>50</v>
+      </c>
+      <c r="B130">
+        <v>4</v>
+      </c>
+      <c r="C130">
+        <v>85</v>
+      </c>
+      <c r="D130">
+        <v>105</v>
+      </c>
+      <c r="E130">
+        <v>65</v>
+      </c>
+      <c r="F130">
+        <v>20</v>
+      </c>
+      <c r="G130">
+        <v>0</v>
+      </c>
+      <c r="H130">
+        <v>2</v>
+      </c>
+      <c r="I130" s="1">
+        <v>1.7592592592592594E-2</v>
+      </c>
+      <c r="J130">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A131" t="s">
+        <v>50</v>
+      </c>
+      <c r="B131">
+        <v>5</v>
+      </c>
+      <c r="C131">
+        <v>105</v>
+      </c>
+      <c r="D131">
+        <v>135</v>
+      </c>
+      <c r="E131">
+        <v>80</v>
+      </c>
+      <c r="F131">
+        <v>25</v>
+      </c>
+      <c r="G131">
+        <v>0</v>
+      </c>
+      <c r="H131">
+        <v>2</v>
+      </c>
+      <c r="I131" s="1">
+        <v>2.3842592592592592E-2</v>
+      </c>
+      <c r="J131">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A132" t="s">
+        <v>50</v>
+      </c>
+      <c r="B132">
+        <v>6</v>
+      </c>
+      <c r="C132">
+        <v>135</v>
+      </c>
+      <c r="D132">
+        <v>170</v>
+      </c>
+      <c r="E132">
+        <v>105</v>
+      </c>
+      <c r="F132">
+        <v>35</v>
+      </c>
+      <c r="G132">
+        <v>1</v>
+      </c>
+      <c r="H132">
+        <v>3</v>
+      </c>
+      <c r="I132" s="1">
+        <v>3.1134259259259261E-2</v>
+      </c>
+      <c r="J132">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A133" t="s">
+        <v>50</v>
+      </c>
+      <c r="B133">
+        <v>7</v>
+      </c>
+      <c r="C133">
+        <v>175</v>
+      </c>
+      <c r="D133">
+        <v>220</v>
+      </c>
+      <c r="E133">
+        <v>130</v>
+      </c>
+      <c r="F133">
+        <v>45</v>
+      </c>
+      <c r="G133">
+        <v>2</v>
+      </c>
+      <c r="H133">
+        <v>4</v>
+      </c>
+      <c r="I133" s="1">
+        <v>3.9583333333333331E-2</v>
+      </c>
+      <c r="J133">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A134" t="s">
+        <v>50</v>
+      </c>
+      <c r="B134">
+        <v>8</v>
+      </c>
+      <c r="C134">
+        <v>225</v>
+      </c>
+      <c r="D134">
+        <v>280</v>
+      </c>
+      <c r="E134">
+        <v>170</v>
+      </c>
+      <c r="F134">
+        <v>55</v>
+      </c>
+      <c r="G134">
+        <v>3</v>
+      </c>
+      <c r="H134">
+        <v>4</v>
+      </c>
+      <c r="I134" s="1">
+        <v>4.9421296296296297E-2</v>
+      </c>
+      <c r="J134">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A135" t="s">
+        <v>50</v>
+      </c>
+      <c r="B135">
+        <v>9</v>
+      </c>
+      <c r="C135">
+        <v>290</v>
+      </c>
+      <c r="D135">
+        <v>360</v>
+      </c>
+      <c r="E135">
+        <v>215</v>
+      </c>
+      <c r="F135">
+        <v>70</v>
+      </c>
+      <c r="G135">
+        <v>4</v>
+      </c>
+      <c r="H135">
+        <v>5</v>
+      </c>
+      <c r="I135" s="1">
+        <v>6.0879629629629631E-2</v>
+      </c>
+      <c r="J135">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A136" t="s">
+        <v>50</v>
+      </c>
+      <c r="B136">
+        <v>10</v>
+      </c>
+      <c r="C136">
+        <v>370</v>
+      </c>
+      <c r="D136">
+        <v>460</v>
+      </c>
+      <c r="E136">
+        <v>275</v>
+      </c>
+      <c r="F136">
+        <v>90</v>
+      </c>
+      <c r="G136">
+        <v>5</v>
+      </c>
+      <c r="H136">
+        <v>6</v>
+      </c>
+      <c r="I136" s="1">
+        <v>7.407407407407407E-2</v>
+      </c>
+      <c r="J136">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
making some tweaks to building structure
</commit_message>
<xml_diff>
--- a/Raw_Building_Data.xlsx
+++ b/Raw_Building_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pyeac\Desktop\Travian Sim V2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BB2CCB3-7E5F-4C1B-8868-6FBC7E6C0506}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8692D5FA-59D8-495B-9726-4A2EC766C129}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{D964349E-A6D7-42EF-9507-D8E4572606D0}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="61">
   <si>
     <t>Building</t>
   </si>
@@ -218,6 +218,9 @@
   <si>
     <t>pop</t>
   </si>
+  <si>
+    <t>Main Building</t>
+  </si>
 </sst>
 </file>
 
@@ -252,11 +255,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2865,10 +2869,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{559C895B-DEBC-4F15-AD65-1EAADE192C37}">
-  <dimension ref="A1:J136"/>
+  <dimension ref="A1:J196"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A164" workbookViewId="0">
+      <selection activeCell="K171" sqref="K171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7228,6 +7232,1926 @@
         <v>1000</v>
       </c>
     </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A137" t="s">
+        <v>11</v>
+      </c>
+      <c r="B137">
+        <v>1</v>
+      </c>
+      <c r="C137">
+        <v>80</v>
+      </c>
+      <c r="D137">
+        <v>100</v>
+      </c>
+      <c r="E137">
+        <v>70</v>
+      </c>
+      <c r="F137">
+        <v>20</v>
+      </c>
+      <c r="G137">
+        <v>1</v>
+      </c>
+      <c r="H137">
+        <v>1</v>
+      </c>
+      <c r="I137" s="1">
+        <v>1.8518518518518517E-2</v>
+      </c>
+      <c r="J137">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A138" t="s">
+        <v>11</v>
+      </c>
+      <c r="B138">
+        <v>2</v>
+      </c>
+      <c r="C138">
+        <v>100</v>
+      </c>
+      <c r="D138">
+        <v>130</v>
+      </c>
+      <c r="E138">
+        <v>90</v>
+      </c>
+      <c r="F138">
+        <v>25</v>
+      </c>
+      <c r="G138">
+        <v>2</v>
+      </c>
+      <c r="H138">
+        <v>1</v>
+      </c>
+      <c r="I138" s="1">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="J138">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A139" t="s">
+        <v>11</v>
+      </c>
+      <c r="B139">
+        <v>3</v>
+      </c>
+      <c r="C139">
+        <v>130</v>
+      </c>
+      <c r="D139">
+        <v>165</v>
+      </c>
+      <c r="E139">
+        <v>115</v>
+      </c>
+      <c r="F139">
+        <v>35</v>
+      </c>
+      <c r="G139">
+        <v>3</v>
+      </c>
+      <c r="H139">
+        <v>2</v>
+      </c>
+      <c r="I139" s="1">
+        <v>3.2407407407407406E-2</v>
+      </c>
+      <c r="J139">
+        <v>2300</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
+        <v>11</v>
+      </c>
+      <c r="B140">
+        <v>4</v>
+      </c>
+      <c r="C140">
+        <v>170</v>
+      </c>
+      <c r="D140">
+        <v>210</v>
+      </c>
+      <c r="E140">
+        <v>145</v>
+      </c>
+      <c r="F140">
+        <v>40</v>
+      </c>
+      <c r="G140">
+        <v>4</v>
+      </c>
+      <c r="H140">
+        <v>2</v>
+      </c>
+      <c r="I140" s="1">
+        <v>4.1087962962962965E-2</v>
+      </c>
+      <c r="J140">
+        <v>3100</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A141" t="s">
+        <v>11</v>
+      </c>
+      <c r="B141">
+        <v>5</v>
+      </c>
+      <c r="C141">
+        <v>215</v>
+      </c>
+      <c r="D141">
+        <v>270</v>
+      </c>
+      <c r="E141">
+        <v>190</v>
+      </c>
+      <c r="F141">
+        <v>55</v>
+      </c>
+      <c r="G141">
+        <v>5</v>
+      </c>
+      <c r="H141">
+        <v>2</v>
+      </c>
+      <c r="I141" s="1">
+        <v>5.1157407407407408E-2</v>
+      </c>
+      <c r="J141">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A142" t="s">
+        <v>11</v>
+      </c>
+      <c r="B142">
+        <v>6</v>
+      </c>
+      <c r="C142">
+        <v>275</v>
+      </c>
+      <c r="D142">
+        <v>345</v>
+      </c>
+      <c r="E142">
+        <v>240</v>
+      </c>
+      <c r="F142">
+        <v>70</v>
+      </c>
+      <c r="G142">
+        <v>6</v>
+      </c>
+      <c r="H142">
+        <v>3</v>
+      </c>
+      <c r="I142" s="1">
+        <v>6.2731481481481485E-2</v>
+      </c>
+      <c r="J142">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A143" t="s">
+        <v>11</v>
+      </c>
+      <c r="B143">
+        <v>7</v>
+      </c>
+      <c r="C143">
+        <v>350</v>
+      </c>
+      <c r="D143">
+        <v>440</v>
+      </c>
+      <c r="E143">
+        <v>310</v>
+      </c>
+      <c r="F143">
+        <v>90</v>
+      </c>
+      <c r="G143">
+        <v>7</v>
+      </c>
+      <c r="H143">
+        <v>4</v>
+      </c>
+      <c r="I143" s="1">
+        <v>7.6273148148148145E-2</v>
+      </c>
+      <c r="J143">
+        <v>6300</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A144" t="s">
+        <v>11</v>
+      </c>
+      <c r="B144">
+        <v>8</v>
+      </c>
+      <c r="C144">
+        <v>450</v>
+      </c>
+      <c r="D144">
+        <v>565</v>
+      </c>
+      <c r="E144">
+        <v>395</v>
+      </c>
+      <c r="F144">
+        <v>115</v>
+      </c>
+      <c r="G144">
+        <v>8</v>
+      </c>
+      <c r="H144">
+        <v>4</v>
+      </c>
+      <c r="I144" s="1">
+        <v>9.2013888888888895E-2</v>
+      </c>
+      <c r="J144">
+        <v>7800</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A145" t="s">
+        <v>11</v>
+      </c>
+      <c r="B145">
+        <v>9</v>
+      </c>
+      <c r="C145">
+        <v>575</v>
+      </c>
+      <c r="D145">
+        <v>720</v>
+      </c>
+      <c r="E145">
+        <v>505</v>
+      </c>
+      <c r="F145">
+        <v>145</v>
+      </c>
+      <c r="G145">
+        <v>9</v>
+      </c>
+      <c r="H145">
+        <v>5</v>
+      </c>
+      <c r="I145" s="1">
+        <v>0.11018518518518519</v>
+      </c>
+      <c r="J145">
+        <v>9600</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A146" t="s">
+        <v>11</v>
+      </c>
+      <c r="B146">
+        <v>10</v>
+      </c>
+      <c r="C146">
+        <v>740</v>
+      </c>
+      <c r="D146">
+        <v>920</v>
+      </c>
+      <c r="E146">
+        <v>645</v>
+      </c>
+      <c r="F146">
+        <v>185</v>
+      </c>
+      <c r="G146">
+        <v>10</v>
+      </c>
+      <c r="H146">
+        <v>6</v>
+      </c>
+      <c r="I146" s="1">
+        <v>0.13125000000000001</v>
+      </c>
+      <c r="J146">
+        <v>11800</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A147" t="s">
+        <v>11</v>
+      </c>
+      <c r="B147">
+        <v>11</v>
+      </c>
+      <c r="C147">
+        <v>945</v>
+      </c>
+      <c r="D147">
+        <v>1180</v>
+      </c>
+      <c r="E147">
+        <v>825</v>
+      </c>
+      <c r="F147">
+        <v>235</v>
+      </c>
+      <c r="G147">
+        <v>12</v>
+      </c>
+      <c r="H147">
+        <v>7</v>
+      </c>
+      <c r="I147" s="1">
+        <v>0.15567129629629631</v>
+      </c>
+      <c r="J147">
+        <v>14400</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A148" t="s">
+        <v>11</v>
+      </c>
+      <c r="B148">
+        <v>12</v>
+      </c>
+      <c r="C148">
+        <v>1210</v>
+      </c>
+      <c r="D148">
+        <v>1510</v>
+      </c>
+      <c r="E148">
+        <v>1060</v>
+      </c>
+      <c r="F148">
+        <v>300</v>
+      </c>
+      <c r="G148">
+        <v>14</v>
+      </c>
+      <c r="H148">
+        <v>9</v>
+      </c>
+      <c r="I148" s="1">
+        <v>0.18414351851851851</v>
+      </c>
+      <c r="J148">
+        <v>17600</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A149" t="s">
+        <v>11</v>
+      </c>
+      <c r="B149">
+        <v>13</v>
+      </c>
+      <c r="C149">
+        <v>1545</v>
+      </c>
+      <c r="D149">
+        <v>1935</v>
+      </c>
+      <c r="E149">
+        <v>1355</v>
+      </c>
+      <c r="F149">
+        <v>385</v>
+      </c>
+      <c r="G149">
+        <v>16</v>
+      </c>
+      <c r="H149">
+        <v>11</v>
+      </c>
+      <c r="I149" s="1">
+        <v>0.2170138888888889</v>
+      </c>
+      <c r="J149">
+        <v>21400</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A150" t="s">
+        <v>11</v>
+      </c>
+      <c r="B150">
+        <v>14</v>
+      </c>
+      <c r="C150">
+        <v>1980</v>
+      </c>
+      <c r="D150">
+        <v>2475</v>
+      </c>
+      <c r="E150">
+        <v>1735</v>
+      </c>
+      <c r="F150">
+        <v>495</v>
+      </c>
+      <c r="G150">
+        <v>18</v>
+      </c>
+      <c r="H150">
+        <v>13</v>
+      </c>
+      <c r="I150" s="1">
+        <v>0.25520833333333331</v>
+      </c>
+      <c r="J150">
+        <v>25900</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A151" t="s">
+        <v>11</v>
+      </c>
+      <c r="B151">
+        <v>15</v>
+      </c>
+      <c r="C151">
+        <v>2535</v>
+      </c>
+      <c r="D151">
+        <v>3170</v>
+      </c>
+      <c r="E151">
+        <v>2220</v>
+      </c>
+      <c r="F151">
+        <v>635</v>
+      </c>
+      <c r="G151">
+        <v>20</v>
+      </c>
+      <c r="H151">
+        <v>15</v>
+      </c>
+      <c r="I151" s="1">
+        <v>0.29953703703703705</v>
+      </c>
+      <c r="J151">
+        <v>31300</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A152" t="s">
+        <v>11</v>
+      </c>
+      <c r="B152">
+        <v>16</v>
+      </c>
+      <c r="C152">
+        <v>3245</v>
+      </c>
+      <c r="D152">
+        <v>4055</v>
+      </c>
+      <c r="E152">
+        <v>2840</v>
+      </c>
+      <c r="F152">
+        <v>810</v>
+      </c>
+      <c r="G152">
+        <v>22</v>
+      </c>
+      <c r="H152">
+        <v>18</v>
+      </c>
+      <c r="I152" s="1">
+        <v>0.35092592592592592</v>
+      </c>
+      <c r="J152">
+        <v>37900</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A153" t="s">
+        <v>11</v>
+      </c>
+      <c r="B153">
+        <v>17</v>
+      </c>
+      <c r="C153">
+        <v>4155</v>
+      </c>
+      <c r="D153">
+        <v>5190</v>
+      </c>
+      <c r="E153">
+        <v>3635</v>
+      </c>
+      <c r="F153">
+        <v>1040</v>
+      </c>
+      <c r="G153">
+        <v>24</v>
+      </c>
+      <c r="H153">
+        <v>22</v>
+      </c>
+      <c r="I153" s="1">
+        <v>0.41053240740740743</v>
+      </c>
+      <c r="J153">
+        <v>45700</v>
+      </c>
+    </row>
+    <row r="154" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A154" t="s">
+        <v>11</v>
+      </c>
+      <c r="B154">
+        <v>18</v>
+      </c>
+      <c r="C154">
+        <v>5315</v>
+      </c>
+      <c r="D154">
+        <v>6645</v>
+      </c>
+      <c r="E154">
+        <v>4650</v>
+      </c>
+      <c r="F154">
+        <v>1330</v>
+      </c>
+      <c r="G154">
+        <v>26</v>
+      </c>
+      <c r="H154">
+        <v>27</v>
+      </c>
+      <c r="I154" s="1">
+        <v>0.47974537037037035</v>
+      </c>
+      <c r="J154">
+        <v>55100</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A155" t="s">
+        <v>11</v>
+      </c>
+      <c r="B155">
+        <v>19</v>
+      </c>
+      <c r="C155">
+        <v>6805</v>
+      </c>
+      <c r="D155">
+        <v>8505</v>
+      </c>
+      <c r="E155">
+        <v>5955</v>
+      </c>
+      <c r="F155">
+        <v>1700</v>
+      </c>
+      <c r="G155">
+        <v>28</v>
+      </c>
+      <c r="H155">
+        <v>32</v>
+      </c>
+      <c r="I155" s="1">
+        <v>0.55995370370370368</v>
+      </c>
+      <c r="J155">
+        <v>66400</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A156" t="s">
+        <v>11</v>
+      </c>
+      <c r="B156">
+        <v>20</v>
+      </c>
+      <c r="C156">
+        <v>8710</v>
+      </c>
+      <c r="D156">
+        <v>10890</v>
+      </c>
+      <c r="E156">
+        <v>7620</v>
+      </c>
+      <c r="F156">
+        <v>2180</v>
+      </c>
+      <c r="G156">
+        <v>30</v>
+      </c>
+      <c r="H156">
+        <v>38</v>
+      </c>
+      <c r="I156" s="1">
+        <v>0.65300925925925923</v>
+      </c>
+      <c r="J156">
+        <v>80000</v>
+      </c>
+    </row>
+    <row r="157" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A157" t="s">
+        <v>10</v>
+      </c>
+      <c r="B157">
+        <v>1</v>
+      </c>
+      <c r="C157">
+        <v>130</v>
+      </c>
+      <c r="D157">
+        <v>160</v>
+      </c>
+      <c r="E157">
+        <v>90</v>
+      </c>
+      <c r="F157">
+        <v>40</v>
+      </c>
+      <c r="G157">
+        <v>1</v>
+      </c>
+      <c r="H157">
+        <v>1</v>
+      </c>
+      <c r="I157" s="1">
+        <v>2.3148148148148147E-2</v>
+      </c>
+      <c r="J157">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A158" t="s">
+        <v>10</v>
+      </c>
+      <c r="B158">
+        <v>2</v>
+      </c>
+      <c r="C158">
+        <v>165</v>
+      </c>
+      <c r="D158">
+        <v>205</v>
+      </c>
+      <c r="E158">
+        <v>115</v>
+      </c>
+      <c r="F158">
+        <v>50</v>
+      </c>
+      <c r="G158">
+        <v>2</v>
+      </c>
+      <c r="H158">
+        <v>1</v>
+      </c>
+      <c r="I158" s="1">
+        <v>3.0324074074074073E-2</v>
+      </c>
+      <c r="J158">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="159" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A159" t="s">
+        <v>10</v>
+      </c>
+      <c r="B159">
+        <v>3</v>
+      </c>
+      <c r="C159">
+        <v>215</v>
+      </c>
+      <c r="D159">
+        <v>260</v>
+      </c>
+      <c r="E159">
+        <v>145</v>
+      </c>
+      <c r="F159">
+        <v>65</v>
+      </c>
+      <c r="G159">
+        <v>3</v>
+      </c>
+      <c r="H159">
+        <v>2</v>
+      </c>
+      <c r="I159" s="1">
+        <v>3.8657407407407404E-2</v>
+      </c>
+      <c r="J159">
+        <v>2300</v>
+      </c>
+    </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A160" t="s">
+        <v>10</v>
+      </c>
+      <c r="B160">
+        <v>4</v>
+      </c>
+      <c r="C160">
+        <v>275</v>
+      </c>
+      <c r="D160">
+        <v>335</v>
+      </c>
+      <c r="E160">
+        <v>190</v>
+      </c>
+      <c r="F160">
+        <v>85</v>
+      </c>
+      <c r="G160">
+        <v>4</v>
+      </c>
+      <c r="H160">
+        <v>2</v>
+      </c>
+      <c r="I160" s="1">
+        <v>4.8263888888888891E-2</v>
+      </c>
+      <c r="J160">
+        <v>3100</v>
+      </c>
+    </row>
+    <row r="161" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A161" t="s">
+        <v>10</v>
+      </c>
+      <c r="B161">
+        <v>5</v>
+      </c>
+      <c r="C161">
+        <v>350</v>
+      </c>
+      <c r="D161">
+        <v>430</v>
+      </c>
+      <c r="E161">
+        <v>240</v>
+      </c>
+      <c r="F161">
+        <v>105</v>
+      </c>
+      <c r="G161">
+        <v>5</v>
+      </c>
+      <c r="H161">
+        <v>2</v>
+      </c>
+      <c r="I161" s="1">
+        <v>5.949074074074074E-2</v>
+      </c>
+      <c r="J161">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="162" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A162" t="s">
+        <v>10</v>
+      </c>
+      <c r="B162">
+        <v>6</v>
+      </c>
+      <c r="C162">
+        <v>445</v>
+      </c>
+      <c r="D162">
+        <v>550</v>
+      </c>
+      <c r="E162">
+        <v>310</v>
+      </c>
+      <c r="F162">
+        <v>135</v>
+      </c>
+      <c r="G162">
+        <v>6</v>
+      </c>
+      <c r="H162">
+        <v>3</v>
+      </c>
+      <c r="I162" s="1">
+        <v>7.2453703703703701E-2</v>
+      </c>
+      <c r="J162">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="163" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A163" t="s">
+        <v>10</v>
+      </c>
+      <c r="B163">
+        <v>7</v>
+      </c>
+      <c r="C163">
+        <v>570</v>
+      </c>
+      <c r="D163">
+        <v>705</v>
+      </c>
+      <c r="E163">
+        <v>395</v>
+      </c>
+      <c r="F163">
+        <v>175</v>
+      </c>
+      <c r="G163">
+        <v>7</v>
+      </c>
+      <c r="H163">
+        <v>4</v>
+      </c>
+      <c r="I163" s="1">
+        <v>8.7615740740740744E-2</v>
+      </c>
+      <c r="J163">
+        <v>6300</v>
+      </c>
+    </row>
+    <row r="164" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A164" t="s">
+        <v>10</v>
+      </c>
+      <c r="B164">
+        <v>8</v>
+      </c>
+      <c r="C164">
+        <v>730</v>
+      </c>
+      <c r="D164">
+        <v>900</v>
+      </c>
+      <c r="E164">
+        <v>505</v>
+      </c>
+      <c r="F164">
+        <v>225</v>
+      </c>
+      <c r="G164">
+        <v>8</v>
+      </c>
+      <c r="H164">
+        <v>4</v>
+      </c>
+      <c r="I164" s="1">
+        <v>0.1050925925925926</v>
+      </c>
+      <c r="J164">
+        <v>7800</v>
+      </c>
+    </row>
+    <row r="165" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A165" t="s">
+        <v>10</v>
+      </c>
+      <c r="B165">
+        <v>9</v>
+      </c>
+      <c r="C165">
+        <v>935</v>
+      </c>
+      <c r="D165">
+        <v>1155</v>
+      </c>
+      <c r="E165">
+        <v>650</v>
+      </c>
+      <c r="F165">
+        <v>290</v>
+      </c>
+      <c r="G165">
+        <v>9</v>
+      </c>
+      <c r="H165">
+        <v>5</v>
+      </c>
+      <c r="I165" s="1">
+        <v>0.12534722222222222</v>
+      </c>
+      <c r="J165">
+        <v>9600</v>
+      </c>
+    </row>
+    <row r="166" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A166" t="s">
+        <v>10</v>
+      </c>
+      <c r="B166">
+        <v>10</v>
+      </c>
+      <c r="C166">
+        <v>1200</v>
+      </c>
+      <c r="D166">
+        <v>1475</v>
+      </c>
+      <c r="E166">
+        <v>830</v>
+      </c>
+      <c r="F166">
+        <v>370</v>
+      </c>
+      <c r="G166">
+        <v>10</v>
+      </c>
+      <c r="H166">
+        <v>6</v>
+      </c>
+      <c r="I166" s="1">
+        <v>0.14884259259259258</v>
+      </c>
+      <c r="J166">
+        <v>11800</v>
+      </c>
+    </row>
+    <row r="167" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A167" t="s">
+        <v>10</v>
+      </c>
+      <c r="B167">
+        <v>11</v>
+      </c>
+      <c r="C167">
+        <v>1535</v>
+      </c>
+      <c r="D167">
+        <v>1890</v>
+      </c>
+      <c r="E167">
+        <v>1065</v>
+      </c>
+      <c r="F167">
+        <v>470</v>
+      </c>
+      <c r="G167">
+        <v>12</v>
+      </c>
+      <c r="H167">
+        <v>7</v>
+      </c>
+      <c r="I167" s="1">
+        <v>0.1761574074074074</v>
+      </c>
+      <c r="J167">
+        <v>14400</v>
+      </c>
+    </row>
+    <row r="168" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A168" t="s">
+        <v>10</v>
+      </c>
+      <c r="B168">
+        <v>12</v>
+      </c>
+      <c r="C168">
+        <v>1965</v>
+      </c>
+      <c r="D168">
+        <v>2420</v>
+      </c>
+      <c r="E168">
+        <v>1360</v>
+      </c>
+      <c r="F168">
+        <v>605</v>
+      </c>
+      <c r="G168">
+        <v>14</v>
+      </c>
+      <c r="H168">
+        <v>9</v>
+      </c>
+      <c r="I168" s="1">
+        <v>0.20775462962962962</v>
+      </c>
+      <c r="J168">
+        <v>17600</v>
+      </c>
+    </row>
+    <row r="169" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A169" t="s">
+        <v>10</v>
+      </c>
+      <c r="B169">
+        <v>13</v>
+      </c>
+      <c r="C169">
+        <v>2515</v>
+      </c>
+      <c r="D169">
+        <v>3095</v>
+      </c>
+      <c r="E169">
+        <v>1740</v>
+      </c>
+      <c r="F169">
+        <v>775</v>
+      </c>
+      <c r="G169">
+        <v>16</v>
+      </c>
+      <c r="H169">
+        <v>11</v>
+      </c>
+      <c r="I169" s="1">
+        <v>0.24456018518518519</v>
+      </c>
+      <c r="J169">
+        <v>21400</v>
+      </c>
+    </row>
+    <row r="170" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A170" t="s">
+        <v>10</v>
+      </c>
+      <c r="B170">
+        <v>14</v>
+      </c>
+      <c r="C170">
+        <v>3220</v>
+      </c>
+      <c r="D170">
+        <v>3960</v>
+      </c>
+      <c r="E170">
+        <v>2230</v>
+      </c>
+      <c r="F170">
+        <v>990</v>
+      </c>
+      <c r="G170">
+        <v>18</v>
+      </c>
+      <c r="H170">
+        <v>13</v>
+      </c>
+      <c r="I170" s="1">
+        <v>0.28715277777777776</v>
+      </c>
+      <c r="J170">
+        <v>25900</v>
+      </c>
+    </row>
+    <row r="171" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A171" t="s">
+        <v>10</v>
+      </c>
+      <c r="B171">
+        <v>15</v>
+      </c>
+      <c r="C171">
+        <v>4120</v>
+      </c>
+      <c r="D171">
+        <v>5070</v>
+      </c>
+      <c r="E171">
+        <v>2850</v>
+      </c>
+      <c r="F171">
+        <v>1270</v>
+      </c>
+      <c r="G171">
+        <v>20</v>
+      </c>
+      <c r="H171">
+        <v>15</v>
+      </c>
+      <c r="I171" s="1">
+        <v>0.33657407407407408</v>
+      </c>
+      <c r="J171">
+        <v>31300</v>
+      </c>
+    </row>
+    <row r="172" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A172" t="s">
+        <v>10</v>
+      </c>
+      <c r="B172">
+        <v>16</v>
+      </c>
+      <c r="C172">
+        <v>5275</v>
+      </c>
+      <c r="D172">
+        <v>6490</v>
+      </c>
+      <c r="E172">
+        <v>3650</v>
+      </c>
+      <c r="F172">
+        <v>1625</v>
+      </c>
+      <c r="G172">
+        <v>22</v>
+      </c>
+      <c r="H172">
+        <v>18</v>
+      </c>
+      <c r="I172" s="1">
+        <v>0.39386574074074077</v>
+      </c>
+      <c r="J172">
+        <v>37900</v>
+      </c>
+    </row>
+    <row r="173" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A173" t="s">
+        <v>10</v>
+      </c>
+      <c r="B173">
+        <v>17</v>
+      </c>
+      <c r="C173">
+        <v>6750</v>
+      </c>
+      <c r="D173">
+        <v>8310</v>
+      </c>
+      <c r="E173">
+        <v>4675</v>
+      </c>
+      <c r="F173">
+        <v>2075</v>
+      </c>
+      <c r="G173">
+        <v>24</v>
+      </c>
+      <c r="H173">
+        <v>22</v>
+      </c>
+      <c r="I173" s="1">
+        <v>0.46030092592592592</v>
+      </c>
+      <c r="J173">
+        <v>45700</v>
+      </c>
+    </row>
+    <row r="174" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A174" t="s">
+        <v>10</v>
+      </c>
+      <c r="B174">
+        <v>18</v>
+      </c>
+      <c r="C174">
+        <v>8640</v>
+      </c>
+      <c r="D174">
+        <v>10635</v>
+      </c>
+      <c r="E174">
+        <v>5980</v>
+      </c>
+      <c r="F174">
+        <v>2660</v>
+      </c>
+      <c r="G174">
+        <v>26</v>
+      </c>
+      <c r="H174">
+        <v>27</v>
+      </c>
+      <c r="I174" s="1">
+        <v>0.53749999999999998</v>
+      </c>
+      <c r="J174">
+        <v>55100</v>
+      </c>
+    </row>
+    <row r="175" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A175" t="s">
+        <v>10</v>
+      </c>
+      <c r="B175">
+        <v>19</v>
+      </c>
+      <c r="C175">
+        <v>11060</v>
+      </c>
+      <c r="D175">
+        <v>13610</v>
+      </c>
+      <c r="E175">
+        <v>7655</v>
+      </c>
+      <c r="F175">
+        <v>3405</v>
+      </c>
+      <c r="G175">
+        <v>28</v>
+      </c>
+      <c r="H175">
+        <v>32</v>
+      </c>
+      <c r="I175" s="1">
+        <v>0.6269675925925926</v>
+      </c>
+      <c r="J175">
+        <v>66400</v>
+      </c>
+    </row>
+    <row r="176" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A176" t="s">
+        <v>10</v>
+      </c>
+      <c r="B176">
+        <v>20</v>
+      </c>
+      <c r="C176">
+        <v>14155</v>
+      </c>
+      <c r="D176">
+        <v>17420</v>
+      </c>
+      <c r="E176">
+        <v>9800</v>
+      </c>
+      <c r="F176">
+        <v>4355</v>
+      </c>
+      <c r="G176">
+        <v>30</v>
+      </c>
+      <c r="H176">
+        <v>38</v>
+      </c>
+      <c r="I176" s="1">
+        <v>0.73067129629629635</v>
+      </c>
+      <c r="J176">
+        <v>80000</v>
+      </c>
+    </row>
+    <row r="177" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A177" t="s">
+        <v>60</v>
+      </c>
+      <c r="B177">
+        <v>1</v>
+      </c>
+      <c r="C177">
+        <v>70</v>
+      </c>
+      <c r="D177">
+        <v>40</v>
+      </c>
+      <c r="E177">
+        <v>60</v>
+      </c>
+      <c r="F177">
+        <v>20</v>
+      </c>
+      <c r="G177">
+        <v>2</v>
+      </c>
+      <c r="H177">
+        <v>2</v>
+      </c>
+      <c r="I177" s="1">
+        <v>2.8935185185185185E-2</v>
+      </c>
+      <c r="J177" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A178" t="s">
+        <v>60</v>
+      </c>
+      <c r="B178">
+        <v>2</v>
+      </c>
+      <c r="C178">
+        <v>90</v>
+      </c>
+      <c r="D178">
+        <v>50</v>
+      </c>
+      <c r="E178">
+        <v>75</v>
+      </c>
+      <c r="F178">
+        <v>25</v>
+      </c>
+      <c r="G178">
+        <v>3</v>
+      </c>
+      <c r="H178">
+        <v>3</v>
+      </c>
+      <c r="I178" s="1">
+        <v>3.0324074074074073E-2</v>
+      </c>
+      <c r="J178" s="4">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="179" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A179" t="s">
+        <v>60</v>
+      </c>
+      <c r="B179">
+        <v>3</v>
+      </c>
+      <c r="C179">
+        <v>115</v>
+      </c>
+      <c r="D179">
+        <v>65</v>
+      </c>
+      <c r="E179">
+        <v>100</v>
+      </c>
+      <c r="F179">
+        <v>35</v>
+      </c>
+      <c r="G179">
+        <v>4</v>
+      </c>
+      <c r="H179">
+        <v>3</v>
+      </c>
+      <c r="I179" s="1">
+        <v>3.726851851851852E-2</v>
+      </c>
+      <c r="J179" s="4">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="180" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A180" t="s">
+        <v>60</v>
+      </c>
+      <c r="B180">
+        <v>4</v>
+      </c>
+      <c r="C180">
+        <v>145</v>
+      </c>
+      <c r="D180">
+        <v>85</v>
+      </c>
+      <c r="E180">
+        <v>125</v>
+      </c>
+      <c r="F180">
+        <v>40</v>
+      </c>
+      <c r="G180">
+        <v>5</v>
+      </c>
+      <c r="H180">
+        <v>4</v>
+      </c>
+      <c r="I180" s="1">
+        <v>4.490740740740741E-2</v>
+      </c>
+      <c r="J180" s="4">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="181" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A181" t="s">
+        <v>60</v>
+      </c>
+      <c r="B181">
+        <v>5</v>
+      </c>
+      <c r="C181">
+        <v>190</v>
+      </c>
+      <c r="D181">
+        <v>105</v>
+      </c>
+      <c r="E181">
+        <v>160</v>
+      </c>
+      <c r="F181">
+        <v>55</v>
+      </c>
+      <c r="G181">
+        <v>6</v>
+      </c>
+      <c r="H181">
+        <v>5</v>
+      </c>
+      <c r="I181" s="1">
+        <v>5.3356481481481484E-2</v>
+      </c>
+      <c r="J181" s="4">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="182" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A182" t="s">
+        <v>60</v>
+      </c>
+      <c r="B182">
+        <v>6</v>
+      </c>
+      <c r="C182">
+        <v>240</v>
+      </c>
+      <c r="D182">
+        <v>135</v>
+      </c>
+      <c r="E182">
+        <v>205</v>
+      </c>
+      <c r="F182">
+        <v>70</v>
+      </c>
+      <c r="G182">
+        <v>8</v>
+      </c>
+      <c r="H182">
+        <v>6</v>
+      </c>
+      <c r="I182" s="1">
+        <v>6.2615740740740736E-2</v>
+      </c>
+      <c r="J182" s="4">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="183" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A183" t="s">
+        <v>60</v>
+      </c>
+      <c r="B183">
+        <v>7</v>
+      </c>
+      <c r="C183">
+        <v>310</v>
+      </c>
+      <c r="D183">
+        <v>175</v>
+      </c>
+      <c r="E183">
+        <v>265</v>
+      </c>
+      <c r="F183">
+        <v>90</v>
+      </c>
+      <c r="G183">
+        <v>10</v>
+      </c>
+      <c r="H183">
+        <v>7</v>
+      </c>
+      <c r="I183" s="1">
+        <v>7.2916666666666671E-2</v>
+      </c>
+      <c r="J183" s="4">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="184" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A184" t="s">
+        <v>60</v>
+      </c>
+      <c r="B184">
+        <v>8</v>
+      </c>
+      <c r="C184">
+        <v>395</v>
+      </c>
+      <c r="D184">
+        <v>225</v>
+      </c>
+      <c r="E184">
+        <v>340</v>
+      </c>
+      <c r="F184">
+        <v>115</v>
+      </c>
+      <c r="G184">
+        <v>12</v>
+      </c>
+      <c r="H184">
+        <v>9</v>
+      </c>
+      <c r="I184" s="1">
+        <v>8.4259259259259256E-2</v>
+      </c>
+      <c r="J184" s="4">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="185" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A185" t="s">
+        <v>60</v>
+      </c>
+      <c r="B185">
+        <v>9</v>
+      </c>
+      <c r="C185">
+        <v>505</v>
+      </c>
+      <c r="D185">
+        <v>290</v>
+      </c>
+      <c r="E185">
+        <v>430</v>
+      </c>
+      <c r="F185">
+        <v>145</v>
+      </c>
+      <c r="G185">
+        <v>14</v>
+      </c>
+      <c r="H185">
+        <v>10</v>
+      </c>
+      <c r="I185" s="1">
+        <v>9.6990740740740738E-2</v>
+      </c>
+      <c r="J185" s="4">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="186" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A186" t="s">
+        <v>60</v>
+      </c>
+      <c r="B186">
+        <v>10</v>
+      </c>
+      <c r="C186">
+        <v>645</v>
+      </c>
+      <c r="D186">
+        <v>370</v>
+      </c>
+      <c r="E186">
+        <v>555</v>
+      </c>
+      <c r="F186">
+        <v>185</v>
+      </c>
+      <c r="G186">
+        <v>16</v>
+      </c>
+      <c r="H186">
+        <v>12</v>
+      </c>
+      <c r="I186" s="1">
+        <v>0.11099537037037037</v>
+      </c>
+      <c r="J186" s="4">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="187" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A187" t="s">
+        <v>60</v>
+      </c>
+      <c r="B187">
+        <v>11</v>
+      </c>
+      <c r="C187">
+        <v>825</v>
+      </c>
+      <c r="D187">
+        <v>470</v>
+      </c>
+      <c r="E187">
+        <v>710</v>
+      </c>
+      <c r="F187">
+        <v>235</v>
+      </c>
+      <c r="G187">
+        <v>18</v>
+      </c>
+      <c r="H187">
+        <v>15</v>
+      </c>
+      <c r="I187" s="1">
+        <v>0.12662037037037038</v>
+      </c>
+      <c r="J187" s="4">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="188" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A188" t="s">
+        <v>60</v>
+      </c>
+      <c r="B188">
+        <v>12</v>
+      </c>
+      <c r="C188">
+        <v>1060</v>
+      </c>
+      <c r="D188">
+        <v>605</v>
+      </c>
+      <c r="E188">
+        <v>905</v>
+      </c>
+      <c r="F188">
+        <v>300</v>
+      </c>
+      <c r="G188">
+        <v>20</v>
+      </c>
+      <c r="H188">
+        <v>18</v>
+      </c>
+      <c r="I188" s="1">
+        <v>0.14398148148148149</v>
+      </c>
+      <c r="J188" s="4">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="189" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A189" t="s">
+        <v>60</v>
+      </c>
+      <c r="B189">
+        <v>13</v>
+      </c>
+      <c r="C189">
+        <v>1355</v>
+      </c>
+      <c r="D189">
+        <v>775</v>
+      </c>
+      <c r="E189">
+        <v>1160</v>
+      </c>
+      <c r="F189">
+        <v>385</v>
+      </c>
+      <c r="G189">
+        <v>22</v>
+      </c>
+      <c r="H189">
+        <v>21</v>
+      </c>
+      <c r="I189" s="1">
+        <v>0.16342592592592592</v>
+      </c>
+      <c r="J189" s="4">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="190" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A190" t="s">
+        <v>60</v>
+      </c>
+      <c r="B190">
+        <v>14</v>
+      </c>
+      <c r="C190">
+        <v>1735</v>
+      </c>
+      <c r="D190">
+        <v>990</v>
+      </c>
+      <c r="E190">
+        <v>1485</v>
+      </c>
+      <c r="F190">
+        <v>495</v>
+      </c>
+      <c r="G190">
+        <v>24</v>
+      </c>
+      <c r="H190">
+        <v>26</v>
+      </c>
+      <c r="I190" s="1">
+        <v>0.1849537037037037</v>
+      </c>
+      <c r="J190" s="4">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="191" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A191" t="s">
+        <v>60</v>
+      </c>
+      <c r="B191">
+        <v>15</v>
+      </c>
+      <c r="C191">
+        <v>2220</v>
+      </c>
+      <c r="D191">
+        <v>1270</v>
+      </c>
+      <c r="E191">
+        <v>1900</v>
+      </c>
+      <c r="F191">
+        <v>635</v>
+      </c>
+      <c r="G191">
+        <v>26</v>
+      </c>
+      <c r="H191">
+        <v>31</v>
+      </c>
+      <c r="I191" s="1">
+        <v>0.20891203703703703</v>
+      </c>
+      <c r="J191" s="4">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="192" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A192" t="s">
+        <v>60</v>
+      </c>
+      <c r="B192">
+        <v>16</v>
+      </c>
+      <c r="C192">
+        <v>2840</v>
+      </c>
+      <c r="D192">
+        <v>1625</v>
+      </c>
+      <c r="E192">
+        <v>2435</v>
+      </c>
+      <c r="F192">
+        <v>810</v>
+      </c>
+      <c r="G192">
+        <v>29</v>
+      </c>
+      <c r="H192">
+        <v>37</v>
+      </c>
+      <c r="I192" s="1">
+        <v>0.23576388888888888</v>
+      </c>
+      <c r="J192" s="4">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="193" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A193" t="s">
+        <v>60</v>
+      </c>
+      <c r="B193">
+        <v>17</v>
+      </c>
+      <c r="C193">
+        <v>3635</v>
+      </c>
+      <c r="D193">
+        <v>2075</v>
+      </c>
+      <c r="E193">
+        <v>3115</v>
+      </c>
+      <c r="F193">
+        <v>1040</v>
+      </c>
+      <c r="G193">
+        <v>32</v>
+      </c>
+      <c r="H193">
+        <v>44</v>
+      </c>
+      <c r="I193" s="1">
+        <v>0.265625</v>
+      </c>
+      <c r="J193" s="4">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="194" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A194" t="s">
+        <v>60</v>
+      </c>
+      <c r="B194">
+        <v>18</v>
+      </c>
+      <c r="C194">
+        <v>4650</v>
+      </c>
+      <c r="D194">
+        <v>2660</v>
+      </c>
+      <c r="E194">
+        <v>3990</v>
+      </c>
+      <c r="F194">
+        <v>1330</v>
+      </c>
+      <c r="G194">
+        <v>35</v>
+      </c>
+      <c r="H194">
+        <v>53</v>
+      </c>
+      <c r="I194" s="1">
+        <v>0.29895833333333333</v>
+      </c>
+      <c r="J194" s="4">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="195" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A195" t="s">
+        <v>60</v>
+      </c>
+      <c r="B195">
+        <v>19</v>
+      </c>
+      <c r="C195">
+        <v>5955</v>
+      </c>
+      <c r="D195">
+        <v>3405</v>
+      </c>
+      <c r="E195">
+        <v>5105</v>
+      </c>
+      <c r="F195">
+        <v>1700</v>
+      </c>
+      <c r="G195">
+        <v>38</v>
+      </c>
+      <c r="H195">
+        <v>64</v>
+      </c>
+      <c r="I195" s="1">
+        <v>0.33611111111111114</v>
+      </c>
+      <c r="J195" s="4">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="196" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A196" t="s">
+        <v>60</v>
+      </c>
+      <c r="B196">
+        <v>20</v>
+      </c>
+      <c r="C196">
+        <v>7620</v>
+      </c>
+      <c r="D196">
+        <v>4355</v>
+      </c>
+      <c r="E196">
+        <v>6535</v>
+      </c>
+      <c r="F196">
+        <v>2180</v>
+      </c>
+      <c r="G196">
+        <v>41</v>
+      </c>
+      <c r="H196">
+        <v>77</v>
+      </c>
+      <c r="I196" s="1">
+        <v>0.37766203703703705</v>
+      </c>
+      <c r="J196" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>